<commit_message>
Added Critical, Added critchance property to spells, styleMods
added with .checkCrit (protected member of Spell)
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -108,13 +108,13 @@
     <t>tanuki_mario</t>
   </si>
   <si>
-    <t>poke</t>
-  </si>
-  <si>
     <t>bolt wk/res</t>
   </si>
   <si>
-    <t>whiff</t>
+    <t>aimed</t>
+  </si>
+  <si>
+    <t>weakpnt</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1020,7 +1020,7 @@
         <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O1" t="s">
         <v>11</v>
@@ -1094,7 +1094,7 @@
         <v>19</v>
       </c>
       <c r="R2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="S2" t="s">
         <v>19</v>
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="P3" t="s">
         <v>19</v>
@@ -1165,7 +1165,7 @@
         <v>19</v>
       </c>
       <c r="T3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="U3" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
finished adding the combat formula (except buffs/debuffs) , revamped the crit formula, redid the ACC stat and hit/miss, Gave style mods + and * modifiers, and added a bunch of style keywords for testing
added + and * modifiers for style mods (so the can be additave and/or multiplicative) added several style keywords for testing (see spellDict)
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -39,9 +39,6 @@
     <t>SPEED</t>
   </si>
   <si>
-    <t>ACC</t>
-  </si>
-  <si>
     <t>EVADE</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>weakpnt</t>
+  </si>
+  <si>
+    <t>ACC (%)</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -993,7 +993,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1005,48 +1005,48 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1058,7 +1058,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1067,7 +1067,7 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -1085,33 +1085,33 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" t="s">
         <v>18</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" t="s">
         <v>19</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>19</v>
-      </c>
-      <c r="R2" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -1123,16 +1123,16 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="H3">
         <v>2.5</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>10</v>
@@ -1150,33 +1150,33 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" t="s">
         <v>19</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T3" t="s">
-        <v>30</v>
-      </c>
-      <c r="U3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -1188,19 +1188,19 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="H4">
         <v>1.5</v>
       </c>
       <c r="I4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>-1</v>
@@ -1215,30 +1215,30 @@
         <v>-2</v>
       </c>
       <c r="O4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" t="s">
         <v>18</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U4" t="s">
         <v>19</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ally damage, stun/stagger,  gauge mechanics, and UI
-Allies are now fully integrated in combat (no custom formula yet though)
-Allies can be stunned/staggered (with custom effect)
-Allies Have gauge mechanics (can only use their assist if gauge is at appropriate level, goes back down to 50%, functions as health in combat, fills over time, and cannot be filled or cast while stunned)
-Allies have UI (using bameter for gauge, and some text objects for name and status)
-Hooked allies up to battle UI (same as enemies for now)
-Fixed targeting bug where spells that should target the right ally target the right enemy instead (inSpellDictionary.cs)
-Removed weakpnt spell from frog (it was super annoying)
-Added teamcrit debug spell that auto-crits both your allies

FILES ADDED

DisplayAlly.cs

FILES MODIFIED

Ally.cs, BattleManager.cs, SpellDictionary.cs MainScene.Unity

(also modified frog)

TODO

add seperate cast level for SUPER (full charge) on allies
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -111,10 +111,10 @@
     <t>aimed</t>
   </si>
   <si>
-    <t>weakpnt</t>
-  </si>
-  <si>
     <t>ACC (%)</t>
+  </si>
+  <si>
+    <t>falchion</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,7 +1005,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
@@ -1094,7 +1094,7 @@
         <v>18</v>
       </c>
       <c r="R2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Added AI module parameters, cleaned up some code
-Added an AI parameters field in the enemy database that can specify any number of parameters to a generic AI module (such as health thresholds, etc.)
-Parameter is in the form of comma-seperated list (in excel)
-Added comments to AI code
-Changed some unclear method names in enemy.cs (timer() -> attackRoutine and setStats -> initialize)
-Cleaned up how spellDictionary is set in enemy

FILES MODIFIED

Enemy.cs, EnemyAI.cs, EnemyDatabase.cs, BattleManager.cs (1 line)
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>HealthLow1</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>75,25</t>
+  </si>
+  <si>
+    <t>AI parameters</t>
   </si>
 </sst>
 </file>
@@ -979,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,21 +1001,22 @@
     <col min="4" max="4" width="11.109375" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
     <col min="11" max="11" width="10.5546875" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" customWidth="1"/>
-    <col min="16" max="16" width="15.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="18" width="11.5546875" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="10" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="19.109375" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" customWidth="1"/>
+    <col min="18" max="18" width="11" customWidth="1"/>
+    <col min="19" max="19" width="11.5546875" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" customWidth="1"/>
+    <col min="22" max="22" width="10" customWidth="1"/>
+    <col min="23" max="23" width="11.33203125" customWidth="1"/>
+    <col min="24" max="24" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1041,43 +1051,46 @@
         <v>37</v>
       </c>
       <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>27</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>14</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1111,44 +1124,47 @@
       <c r="K2" t="s">
         <v>38</v>
       </c>
-      <c r="L2">
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.5</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1.5</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>16</v>
-      </c>
-      <c r="R2" t="s">
-        <v>17</v>
       </c>
       <c r="S2" t="s">
         <v>17</v>
       </c>
       <c r="T2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" t="s">
         <v>30</v>
-      </c>
-      <c r="U2" t="s">
-        <v>17</v>
       </c>
       <c r="V2" t="s">
         <v>17</v>
       </c>
       <c r="W2" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1182,11 +1198,11 @@
       <c r="K3" t="s">
         <v>38</v>
       </c>
-      <c r="L3">
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3">
         <v>1.2</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1194,32 +1210,35 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>20</v>
-      </c>
-      <c r="R3" t="s">
-        <v>17</v>
       </c>
       <c r="S3" t="s">
         <v>17</v>
       </c>
       <c r="T3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" t="s">
         <v>20</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>17</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>28</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1253,56 +1272,59 @@
       <c r="K4" t="s">
         <v>39</v>
       </c>
-      <c r="L4">
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4">
         <v>-1</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>2</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>0.75</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>-2</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>16</v>
-      </c>
-      <c r="R4" t="s">
-        <v>17</v>
       </c>
       <c r="S4" t="s">
         <v>17</v>
       </c>
       <c r="T4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" t="s">
         <v>20</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>22</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>17</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>36</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>34</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>17</v>
       </c>
       <c r="Z4" t="s">
         <v>17</v>
       </c>
       <c r="AA4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Minor Battle Background changes
Fixed some dimming bugs during battle.
Implemented some assets for battles.
Implemented conveyor belt sliding backgrounds.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JTI-PC\unity_projects\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -99,9 +99,6 @@
     <t>frog_mario</t>
   </si>
   <si>
-    <t>tanuki_mario</t>
-  </si>
-  <si>
     <t>bolt wk/res</t>
   </si>
   <si>
@@ -148,6 +145,21 @@
   </si>
   <si>
     <t>AI parameters</t>
+  </si>
+  <si>
+    <t>tanuki</t>
+  </si>
+  <si>
+    <t>Ladon</t>
+  </si>
+  <si>
+    <t>ladon</t>
+  </si>
+  <si>
+    <t>Lilim</t>
+  </si>
+  <si>
+    <t>lilim</t>
   </si>
 </sst>
 </file>
@@ -988,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1039,19 +1051,19 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M1" t="s">
         <v>6</v>
@@ -1063,10 +1075,10 @@
         <v>8</v>
       </c>
       <c r="P1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R1" t="s">
         <v>9</v>
@@ -1087,7 +1099,7 @@
         <v>14</v>
       </c>
       <c r="X1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -1122,10 +1134,10 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -1140,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="Q2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R2" t="s">
         <v>16</v>
@@ -1152,7 +1164,7 @@
         <v>17</v>
       </c>
       <c r="U2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V2" t="s">
         <v>17</v>
@@ -1169,7 +1181,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -1196,10 +1208,10 @@
         <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M3">
         <v>1.2</v>
@@ -1214,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R3" t="s">
         <v>20</v>
@@ -1232,7 +1244,7 @@
         <v>17</v>
       </c>
       <c r="W3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X3" t="s">
         <v>18</v>
@@ -1270,10 +1282,10 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M4">
         <v>-1</v>
@@ -1288,7 +1300,7 @@
         <v>-2</v>
       </c>
       <c r="Q4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R4" t="s">
         <v>16</v>
@@ -1309,10 +1321,10 @@
         <v>17</v>
       </c>
       <c r="X4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Y4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z4" t="s">
         <v>17</v>
@@ -1326,6 +1338,166 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0.95</v>
+      </c>
+      <c r="G5">
+        <v>-0.2</v>
+      </c>
+      <c r="H5">
+        <v>2.5</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5">
+        <v>1.2</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U5" t="s">
+        <v>20</v>
+      </c>
+      <c r="V5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W5" t="s">
+        <v>27</v>
+      </c>
+      <c r="X5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1.25</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>1.5</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6">
+        <v>-1</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>0.75</v>
+      </c>
+      <c r="P6">
+        <v>-2</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" t="s">
+        <v>17</v>
+      </c>
+      <c r="U6" t="s">
+        <v>20</v>
+      </c>
+      <c r="V6" t="s">
+        <v>22</v>
+      </c>
+      <c r="W6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed broken chat database from merge
EnemyDatabase was missing chat database stuff from merge.
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>lilim</t>
+  </si>
+  <si>
+    <t>chat_id</t>
+  </si>
+  <si>
+    <t>enemy_general_1</t>
+  </si>
+  <si>
+    <t>tanooki_1</t>
   </si>
 </sst>
 </file>
@@ -1000,35 +1009,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB7"/>
+  <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" customWidth="1"/>
-    <col min="14" max="14" width="9.88671875" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11" customWidth="1"/>
-    <col min="19" max="19" width="11.5546875" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" customWidth="1"/>
-    <col min="21" max="21" width="11.33203125" customWidth="1"/>
-    <col min="22" max="22" width="10" customWidth="1"/>
-    <col min="23" max="23" width="11.33203125" customWidth="1"/>
-    <col min="24" max="24" width="19.109375" customWidth="1"/>
+    <col min="2" max="3" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
+    <col min="23" max="23" width="10" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" customWidth="1"/>
+    <col min="25" max="25" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1036,188 +1045,206 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>10</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>11</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>12</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>13</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>14</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>1.5</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>37</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>39</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.5</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>1.5</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>1</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>34</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>16</v>
       </c>
-      <c r="S2" t="s">
-        <v>17</v>
-      </c>
       <c r="T2" t="s">
         <v>17</v>
       </c>
       <c r="U2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V2" t="s">
         <v>29</v>
       </c>
-      <c r="V2" t="s">
-        <v>17</v>
-      </c>
       <c r="W2" t="s">
         <v>17</v>
       </c>
       <c r="X2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
         <v>100</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.95</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>-0.2</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>2.5</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>10</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>37</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>39</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1.2</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -1225,159 +1252,177 @@
       <c r="P3">
         <v>1</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
         <v>34</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>20</v>
       </c>
-      <c r="S3" t="s">
-        <v>17</v>
-      </c>
       <c r="T3" t="s">
         <v>17</v>
       </c>
       <c r="U3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V3" t="s">
         <v>20</v>
       </c>
-      <c r="V3" t="s">
-        <v>17</v>
-      </c>
       <c r="W3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X3" t="s">
         <v>27</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4">
         <v>50</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1.25</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.2</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1.5</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>38</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>40</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>-1</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>2</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.75</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>-2</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>34</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>16</v>
       </c>
-      <c r="S4" t="s">
-        <v>17</v>
-      </c>
       <c r="T4" t="s">
         <v>17</v>
       </c>
       <c r="U4" t="s">
+        <v>17</v>
+      </c>
+      <c r="V4" t="s">
         <v>20</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>22</v>
       </c>
-      <c r="W4" t="s">
-        <v>17</v>
-      </c>
       <c r="X4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y4" t="s">
         <v>35</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>33</v>
       </c>
-      <c r="Z4" t="s">
-        <v>17</v>
-      </c>
       <c r="AA4" t="s">
         <v>17</v>
       </c>
       <c r="AB4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5">
         <v>100</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.95</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>-0.2</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>2.5</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>10</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>37</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>39</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1.2</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -1385,118 +1430,136 @@
       <c r="P5">
         <v>1</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
         <v>34</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>20</v>
       </c>
-      <c r="S5" t="s">
-        <v>17</v>
-      </c>
       <c r="T5" t="s">
         <v>17</v>
       </c>
       <c r="U5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V5" t="s">
         <v>20</v>
       </c>
-      <c r="V5" t="s">
-        <v>17</v>
-      </c>
       <c r="W5" t="s">
+        <v>17</v>
+      </c>
+      <c r="X5" t="s">
         <v>27</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6">
         <v>50</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1.25</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.2</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>1.5</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>38</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>40</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>-1</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>2</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.75</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>-2</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>34</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>16</v>
       </c>
-      <c r="S6" t="s">
-        <v>17</v>
-      </c>
       <c r="T6" t="s">
         <v>17</v>
       </c>
       <c r="U6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" t="s">
         <v>20</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>22</v>
       </c>
-      <c r="W6" t="s">
-        <v>17</v>
-      </c>
       <c r="X6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y6" t="s">
         <v>35</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>33</v>
       </c>
-      <c r="Z6" t="s">
-        <v>17</v>
-      </c>
       <c r="AA6" t="s">
         <v>17</v>
       </c>
       <c r="AB6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Lower speed is now slower, higher is faster
casting time = cast_time / speed now
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JTI-PC\unity_projects\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1009,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1559,8 +1559,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added all act 1 enemies and Encounter setup
-Added sprites (most placeholder) for all act1 enemies and enetered their stats into the enemy database.
-Created a playtest-1 gameflow for the playtest that contains all act1 encounters and (don't use this yet the game will crash as there is no doppleganger AI)
-Added spacing to battle gameflow format
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="70">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -111,9 +111,6 @@
     <t>falchion</t>
   </si>
   <si>
-    <t>SPEED (Higher is lower0</t>
-  </si>
-  <si>
     <t>SpellGroup 1</t>
   </si>
   <si>
@@ -147,21 +144,12 @@
     <t>AI parameters</t>
   </si>
   <si>
-    <t>tanuki</t>
-  </si>
-  <si>
     <t>Ladon</t>
   </si>
   <si>
-    <t>ladon</t>
-  </si>
-  <si>
     <t>Lilim</t>
   </si>
   <si>
-    <t>lilim</t>
-  </si>
-  <si>
     <t>chat_id</t>
   </si>
   <si>
@@ -169,6 +157,78 @@
   </si>
   <si>
     <t>tanooki_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPEED </t>
+  </si>
+  <si>
+    <t>Changeling</t>
+  </si>
+  <si>
+    <t>spr_bt_changeling_placeholder</t>
+  </si>
+  <si>
+    <t>spr_bt_tanuki</t>
+  </si>
+  <si>
+    <t>spr_bt_ladon</t>
+  </si>
+  <si>
+    <t>spr_bt_lilim</t>
+  </si>
+  <si>
+    <t>Tanuki2</t>
+  </si>
+  <si>
+    <t>Ijiraq</t>
+  </si>
+  <si>
+    <t>ice</t>
+  </si>
+  <si>
+    <t>spr_bt_ijiraq_placeholder</t>
+  </si>
+  <si>
+    <t>Ijiraq2</t>
+  </si>
+  <si>
+    <t>Doppelganger (BLUE)</t>
+  </si>
+  <si>
+    <t>spr_bt_doppelganger_b_placeholder</t>
+  </si>
+  <si>
+    <t>Doppleganger</t>
+  </si>
+  <si>
+    <t>GROUP/TOO_LONG</t>
+  </si>
+  <si>
+    <t>spr_bt_doppelganger_y_placeholder</t>
+  </si>
+  <si>
+    <t>spr_bt_doppelganger_r_placeholder</t>
+  </si>
+  <si>
+    <t>Doppelganger (RED)</t>
+  </si>
+  <si>
+    <t>Doppelganger (YELLOW)</t>
+  </si>
+  <si>
+    <t>Doppelganger (GRAY)</t>
+  </si>
+  <si>
+    <t>spr_bt_doppelganger_g_placeholder</t>
+  </si>
+  <si>
+    <t>volt</t>
+  </si>
+  <si>
+    <t>GROUP/SPECIAL</t>
+  </si>
+  <si>
+    <t>magic_circle</t>
   </si>
 </sst>
 </file>
@@ -1009,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC8"/>
+  <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AH13" sqref="AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1037,7 +1097,7 @@
     <col min="25" max="25" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1105,7 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1063,7 +1123,7 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="J1" t="s">
         <v>28</v>
@@ -1072,10 +1132,10 @@
         <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N1" t="s">
         <v>6</v>
@@ -1090,7 +1150,7 @@
         <v>26</v>
       </c>
       <c r="R1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S1" t="s">
         <v>9</v>
@@ -1111,10 +1171,10 @@
         <v>14</v>
       </c>
       <c r="Y1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1122,7 +1182,7 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -1140,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="J2">
         <v>1.5</v>
@@ -1149,10 +1209,10 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -1167,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S2" t="s">
         <v>16</v>
@@ -1188,10 +1248,10 @@
         <v>17</v>
       </c>
       <c r="Y2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Z2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA2" t="s">
         <v>17</v>
@@ -1203,39 +1263,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>0.95</v>
+        <v>1.25</v>
       </c>
       <c r="H3">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="I3">
-        <v>2.5</v>
+        <v>0.75</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L3" t="s">
         <v>37</v>
@@ -1244,22 +1304,22 @@
         <v>39</v>
       </c>
       <c r="N3">
-        <v>1.2</v>
+        <v>-1</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="R3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="T3" t="s">
         <v>17</v>
@@ -1271,16 +1331,16 @@
         <v>20</v>
       </c>
       <c r="W3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="X3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="Y3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Z3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA3" t="s">
         <v>17</v>
@@ -1292,63 +1352,63 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>1.25</v>
+        <v>0.95</v>
       </c>
       <c r="H4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="I4">
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
         <v>38</v>
       </c>
-      <c r="M4" t="s">
-        <v>40</v>
-      </c>
       <c r="N4">
-        <v>-1</v>
+        <v>1.2</v>
       </c>
       <c r="O4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="T4" t="s">
         <v>17</v>
@@ -1360,16 +1420,16 @@
         <v>20</v>
       </c>
       <c r="W4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="X4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="Y4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Z4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA4" t="s">
         <v>17</v>
@@ -1381,39 +1441,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
       <c r="D5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>0.95</v>
+        <v>1.25</v>
       </c>
       <c r="H5">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="I5">
-        <v>2.5</v>
+        <v>0.75</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L5" t="s">
         <v>37</v>
@@ -1422,22 +1482,22 @@
         <v>39</v>
       </c>
       <c r="N5">
-        <v>1.2</v>
+        <v>-1</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="R5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="T5" t="s">
         <v>17</v>
@@ -1449,16 +1509,16 @@
         <v>20</v>
       </c>
       <c r="W5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="X5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="Y5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Z5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA5" t="s">
         <v>17</v>
@@ -1470,60 +1530,60 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.5</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
         <v>2</v>
       </c>
-      <c r="G6">
-        <v>1.25</v>
-      </c>
-      <c r="H6">
-        <v>0.2</v>
-      </c>
-      <c r="I6">
-        <v>1.5</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N6">
-        <v>-1</v>
-      </c>
-      <c r="O6">
-        <v>2</v>
-      </c>
-      <c r="P6">
-        <v>0.75</v>
-      </c>
-      <c r="Q6">
-        <v>-2</v>
-      </c>
       <c r="R6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S6" t="s">
         <v>16</v>
@@ -1535,32 +1595,681 @@
         <v>17</v>
       </c>
       <c r="V6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.75</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0.5</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7" t="s">
         <v>20</v>
       </c>
-      <c r="W6" t="s">
+      <c r="T7" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" t="s">
+        <v>17</v>
+      </c>
+      <c r="V7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8">
+        <v>35</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0.85</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>25</v>
+      </c>
+      <c r="L8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0.5</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S8" t="s">
+        <v>16</v>
+      </c>
+      <c r="T8" t="s">
+        <v>17</v>
+      </c>
+      <c r="U8" t="s">
+        <v>17</v>
+      </c>
+      <c r="V8" t="s">
+        <v>20</v>
+      </c>
+      <c r="W8" t="s">
+        <v>17</v>
+      </c>
+      <c r="X8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>1.2</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0.5</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>-1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>33</v>
+      </c>
+      <c r="S9" t="s">
+        <v>16</v>
+      </c>
+      <c r="T9" t="s">
+        <v>17</v>
+      </c>
+      <c r="U9" t="s">
+        <v>17</v>
+      </c>
+      <c r="V9" t="s">
+        <v>16</v>
+      </c>
+      <c r="W9" t="s">
+        <v>54</v>
+      </c>
+      <c r="X9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>65</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1.2</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.6</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>-1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" t="s">
+        <v>54</v>
+      </c>
+      <c r="U10" t="s">
+        <v>17</v>
+      </c>
+      <c r="V10" t="s">
+        <v>16</v>
+      </c>
+      <c r="W10" t="s">
+        <v>54</v>
+      </c>
+      <c r="X10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1.5</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.8</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11">
+        <v>0.5</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>-1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>33</v>
+      </c>
+      <c r="S11" t="s">
+        <v>16</v>
+      </c>
+      <c r="T11" t="s">
+        <v>54</v>
+      </c>
+      <c r="U11" t="s">
+        <v>17</v>
+      </c>
+      <c r="V11" t="s">
+        <v>20</v>
+      </c>
+      <c r="W11" t="s">
+        <v>54</v>
+      </c>
+      <c r="X11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>1.5</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0.8</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12">
+        <v>0.5</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <v>-1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12" t="s">
+        <v>16</v>
+      </c>
+      <c r="T12" t="s">
+        <v>67</v>
+      </c>
+      <c r="U12" t="s">
+        <v>17</v>
+      </c>
+      <c r="V12" t="s">
+        <v>20</v>
+      </c>
+      <c r="W12" t="s">
+        <v>67</v>
+      </c>
+      <c r="X12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>1.5</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0.8</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>59</v>
+      </c>
+      <c r="M13" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13">
+        <v>0.5</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>-1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>33</v>
+      </c>
+      <c r="S13" t="s">
+        <v>16</v>
+      </c>
+      <c r="T13" t="s">
         <v>22</v>
       </c>
-      <c r="X6" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="U13" t="s">
+        <v>17</v>
+      </c>
+      <c r="V13" t="s">
+        <v>20</v>
+      </c>
+      <c r="W13" t="s">
+        <v>22</v>
+      </c>
+      <c r="X13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>1.5</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1.5</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>59</v>
+      </c>
+      <c r="M14" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14">
+        <v>0.5</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>-1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
         <v>33</v>
       </c>
-      <c r="AA6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC6" t="s">
+      <c r="S14" t="s">
+        <v>29</v>
+      </c>
+      <c r="T14" t="s">
+        <v>17</v>
+      </c>
+      <c r="U14" t="s">
+        <v>17</v>
+      </c>
+      <c r="V14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Gameflow issues, fixed spell borking
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -192,43 +192,43 @@
     <t>Ijiraq2</t>
   </si>
   <si>
+    <t>spr_bt_doppelganger_b_placeholder</t>
+  </si>
+  <si>
+    <t>GROUP/TOO_LONG</t>
+  </si>
+  <si>
+    <t>spr_bt_doppelganger_y_placeholder</t>
+  </si>
+  <si>
+    <t>spr_bt_doppelganger_r_placeholder</t>
+  </si>
+  <si>
+    <t>spr_bt_doppelganger_g_placeholder</t>
+  </si>
+  <si>
+    <t>volt</t>
+  </si>
+  <si>
+    <t>GROUP/SPECIAL</t>
+  </si>
+  <si>
+    <t>magic_circle</t>
+  </si>
+  <si>
+    <t>Doppleganger1</t>
+  </si>
+  <si>
     <t>Doppelganger (BLUE)</t>
   </si>
   <si>
-    <t>spr_bt_doppelganger_b_placeholder</t>
-  </si>
-  <si>
-    <t>Doppleganger</t>
-  </si>
-  <si>
-    <t>GROUP/TOO_LONG</t>
-  </si>
-  <si>
-    <t>spr_bt_doppelganger_y_placeholder</t>
-  </si>
-  <si>
-    <t>spr_bt_doppelganger_r_placeholder</t>
+    <t>Doppelganger (YELLOW)</t>
   </si>
   <si>
     <t>Doppelganger (RED)</t>
   </si>
   <si>
-    <t>Doppelganger (YELLOW)</t>
-  </si>
-  <si>
     <t>Doppelganger (GRAY)</t>
-  </si>
-  <si>
-    <t>spr_bt_doppelganger_g_placeholder</t>
-  </si>
-  <si>
-    <t>volt</t>
-  </si>
-  <si>
-    <t>GROUP/SPECIAL</t>
-  </si>
-  <si>
-    <t>magic_circle</t>
   </si>
 </sst>
 </file>
@@ -1071,13 +1071,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AH13" sqref="AH13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="3" width="14.5546875" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
@@ -1899,10 +1899,10 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
       </c>
       <c r="C11" t="s">
         <v>44</v>
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="M11" t="s">
         <v>38</v>
@@ -1971,7 +1971,7 @@
         <v>17</v>
       </c>
       <c r="Y11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Z11" t="s">
         <v>29</v>
@@ -1983,10 +1983,10 @@
         <v>17</v>
       </c>
       <c r="AC11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AD11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AE11" t="s">
         <v>17</v>
@@ -2000,10 +2000,10 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
         <v>44</v>
@@ -2033,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="M12" t="s">
         <v>38</v>
@@ -2057,7 +2057,7 @@
         <v>16</v>
       </c>
       <c r="T12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="U12" t="s">
         <v>17</v>
@@ -2066,28 +2066,28 @@
         <v>20</v>
       </c>
       <c r="W12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="X12" t="s">
         <v>17</v>
       </c>
       <c r="Y12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Z12" t="s">
         <v>29</v>
       </c>
       <c r="AA12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="AB12" t="s">
         <v>17</v>
       </c>
       <c r="AC12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AD12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AE12" t="s">
         <v>17</v>
@@ -2101,10 +2101,10 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
         <v>44</v>
@@ -2134,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="M13" t="s">
         <v>38</v>
@@ -2173,7 +2173,7 @@
         <v>17</v>
       </c>
       <c r="Y13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Z13" t="s">
         <v>29</v>
@@ -2185,10 +2185,10 @@
         <v>17</v>
       </c>
       <c r="AC13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AD13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AE13" t="s">
         <v>17</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
         <v>44</v>
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="M14" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Fixed enemy definitions, removed ally UI when there are no allies, removed crit info when enemy blocks damage
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -1072,7 +1072,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1677,7 +1677,7 @@
         <v>45</v>
       </c>
       <c r="D8">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1784,7 +1784,7 @@
         <v>38</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>2</v>
@@ -1861,7 +1861,7 @@
         <v>38</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10">
         <v>2</v>

</xml_diff>

<commit_message>
Implemented playtest1 gameflow and balancing
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="72">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>Doppelganger (GRAY)</t>
+  </si>
+  <si>
+    <t>Ijiraq3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spear </t>
   </si>
 </sst>
 </file>
@@ -1069,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG15"/>
+  <dimension ref="A1:AG16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1630,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="K7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L7" t="s">
         <v>36</v>
@@ -1754,7 +1760,7 @@
         <v>44</v>
       </c>
       <c r="D9">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1899,31 +1905,31 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
         <v>44</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1932,16 +1938,16 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="M11" t="s">
         <v>38</v>
       </c>
       <c r="N11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O11">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P11">
         <v>-1</v>
@@ -1953,7 +1959,7 @@
         <v>33</v>
       </c>
       <c r="S11" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="T11" t="s">
         <v>54</v>
@@ -1962,7 +1968,7 @@
         <v>17</v>
       </c>
       <c r="V11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="W11" t="s">
         <v>54</v>
@@ -1971,39 +1977,15 @@
         <v>17</v>
       </c>
       <c r="Y11" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>44</v>
@@ -2015,7 +1997,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>1.5</v>
@@ -2057,7 +2039,7 @@
         <v>16</v>
       </c>
       <c r="T12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="U12" t="s">
         <v>17</v>
@@ -2066,7 +2048,7 @@
         <v>20</v>
       </c>
       <c r="W12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="X12" t="s">
         <v>17</v>
@@ -2078,7 +2060,7 @@
         <v>29</v>
       </c>
       <c r="AA12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="AB12" t="s">
         <v>17</v>
@@ -2101,10 +2083,10 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
         <v>44</v>
@@ -2158,7 +2140,7 @@
         <v>16</v>
       </c>
       <c r="T13" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="U13" t="s">
         <v>17</v>
@@ -2167,7 +2149,7 @@
         <v>20</v>
       </c>
       <c r="W13" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="X13" t="s">
         <v>17</v>
@@ -2179,7 +2161,7 @@
         <v>29</v>
       </c>
       <c r="AA13" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="AB13" t="s">
         <v>17</v>
@@ -2202,10 +2184,10 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>44</v>
@@ -2226,7 +2208,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -2256,20 +2238,121 @@
         <v>33</v>
       </c>
       <c r="S14" t="s">
+        <v>16</v>
+      </c>
+      <c r="T14" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" t="s">
+        <v>17</v>
+      </c>
+      <c r="V14" t="s">
+        <v>20</v>
+      </c>
+      <c r="W14" t="s">
+        <v>22</v>
+      </c>
+      <c r="X14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z14" t="s">
         <v>29</v>
       </c>
-      <c r="T14" t="s">
-        <v>17</v>
-      </c>
-      <c r="U14" t="s">
-        <v>17</v>
-      </c>
-      <c r="V14" t="s">
+      <c r="AA14" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>1.5</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1.5</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15">
+        <v>0.5</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>-1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>33</v>
+      </c>
+      <c r="S15" t="s">
+        <v>29</v>
+      </c>
+      <c r="T15" t="s">
+        <v>17</v>
+      </c>
+      <c r="U15" t="s">
+        <v>17</v>
+      </c>
+      <c r="V15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed spellbook arrow layer, Added Doppelganger AI
todo: add functionality for the magic_circle spell

SASUN LIVES!
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hughe\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enemyDatabase" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="76">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -244,12 +244,15 @@
   </si>
   <si>
     <t>doppelganger_1</t>
+  </si>
+  <si>
+    <t>Doppelganger (???)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1083,36 +1086,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="3" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="3" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" customWidth="1"/>
-    <col min="25" max="25" width="19.140625" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" customWidth="1"/>
+    <col min="25" max="25" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +1192,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1367,7 +1370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1456,7 +1459,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1545,7 +1548,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1681,7 +1684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -1989,7 +1992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>74</v>
       </c>
       <c r="D12">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2039,7 +2042,7 @@
         <v>-1</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R12" t="s">
         <v>28</v>
@@ -2090,7 +2093,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>74</v>
       </c>
       <c r="D13">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2134,13 +2137,13 @@
         <v>0.5</v>
       </c>
       <c r="O13">
+        <v>0.5</v>
+      </c>
+      <c r="P13">
         <v>2</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>-1</v>
-      </c>
-      <c r="Q13">
-        <v>1</v>
       </c>
       <c r="R13" t="s">
         <v>28</v>
@@ -2191,7 +2194,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -2202,7 +2205,7 @@
         <v>74</v>
       </c>
       <c r="D14">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2235,13 +2238,13 @@
         <v>0.5</v>
       </c>
       <c r="O14">
+        <v>-1</v>
+      </c>
+      <c r="P14">
+        <v>0.5</v>
+      </c>
+      <c r="Q14">
         <v>2</v>
-      </c>
-      <c r="P14">
-        <v>-1</v>
-      </c>
-      <c r="Q14">
-        <v>1</v>
       </c>
       <c r="R14" t="s">
         <v>28</v>
@@ -2292,39 +2295,39 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
         <v>74</v>
       </c>
       <c r="D15">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G15">
         <v>1.5</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I15">
-        <v>1.5</v>
+        <v>0.95</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L15" t="s">
         <v>58</v>
@@ -2333,22 +2336,22 @@
         <v>33</v>
       </c>
       <c r="N15">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" t="s">
         <v>28</v>
       </c>
       <c r="S15" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="T15" t="s">
         <v>15</v>
@@ -2360,8 +2363,76 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16">
+        <v>75</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M16" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>28</v>
+      </c>
+      <c r="S16" t="s">
+        <v>66</v>
+      </c>
+      <c r="T16" t="s">
+        <v>15</v>
+      </c>
+      <c r="U16" t="s">
+        <v>15</v>
+      </c>
+      <c r="V16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PPU of animations changed, Adjusted SFX Volumes/Reverb, Added Popup stuff
- PPU of animations changed
- Adjusted the volume/reverb of spell sound effects and UI sound effects
- Added temporary "damage number" SFX
- Added color change functionality to damage pop-ups; now healing/negative HP damage displays as "+[value]" in green text
- Updated Changeling sprite
- doppelganger boss muasic file updated to be quieter now
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hughe\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="enemyDatabase" sheetId="1" r:id="rId1"/>
@@ -150,9 +150,6 @@
     <t>Changeling</t>
   </si>
   <si>
-    <t>spr_bt_changeling_placeholder</t>
-  </si>
-  <si>
     <t>spr_bt_tanuki</t>
   </si>
   <si>
@@ -247,12 +244,15 @@
   </si>
   <si>
     <t>Doppelganger (???)</t>
+  </si>
+  <si>
+    <t>spr_bt_changeling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1086,36 +1086,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="3" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" customWidth="1"/>
-    <col min="18" max="18" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="3" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="11.5546875" customWidth="1"/>
-    <col min="21" max="21" width="10.33203125" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="11.33203125" customWidth="1"/>
-    <col min="25" max="25" width="19.109375" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" customWidth="1"/>
+    <col min="25" max="25" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1159,10 +1159,10 @@
         <v>6</v>
       </c>
       <c r="O1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q1" t="s">
         <v>22</v>
@@ -1192,7 +1192,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>15</v>
       </c>
       <c r="V2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W2" t="s">
         <v>15</v>
@@ -1281,7 +1281,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1346,10 +1346,10 @@
         <v>15</v>
       </c>
       <c r="V3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="X3" t="s">
         <v>15</v>
@@ -1370,12 +1370,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -1426,7 +1426,7 @@
         <v>28</v>
       </c>
       <c r="S4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T4" t="s">
         <v>15</v>
@@ -1435,7 +1435,7 @@
         <v>15</v>
       </c>
       <c r="V4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W4" t="s">
         <v>15</v>
@@ -1459,12 +1459,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -1524,10 +1524,10 @@
         <v>15</v>
       </c>
       <c r="V5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="X5" t="s">
         <v>15</v>
@@ -1548,15 +1548,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -1616,12 +1616,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
@@ -1672,7 +1672,7 @@
         <v>28</v>
       </c>
       <c r="S7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T7" t="s">
         <v>15</v>
@@ -1684,12 +1684,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
         <v>40</v>
@@ -1749,7 +1749,7 @@
         <v>15</v>
       </c>
       <c r="V8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W8" t="s">
         <v>15</v>
@@ -1761,15 +1761,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9">
         <v>20</v>
@@ -1829,7 +1829,7 @@
         <v>14</v>
       </c>
       <c r="W9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X9" t="s">
         <v>15</v>
@@ -1838,15 +1838,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>65</v>
@@ -1894,10 +1894,10 @@
         <v>28</v>
       </c>
       <c r="S10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U10" t="s">
         <v>15</v>
@@ -1906,7 +1906,7 @@
         <v>14</v>
       </c>
       <c r="W10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X10" t="s">
         <v>15</v>
@@ -1915,15 +1915,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>45</v>
@@ -1971,10 +1971,10 @@
         <v>28</v>
       </c>
       <c r="S11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U11" t="s">
         <v>15</v>
@@ -1983,7 +1983,7 @@
         <v>14</v>
       </c>
       <c r="W11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X11" t="s">
         <v>15</v>
@@ -1992,15 +1992,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12">
         <v>150</v>
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M12" t="s">
         <v>33</v>
@@ -2051,37 +2051,37 @@
         <v>14</v>
       </c>
       <c r="T12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U12" t="s">
         <v>15</v>
       </c>
       <c r="V12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X12" t="s">
         <v>15</v>
       </c>
       <c r="Y12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB12" t="s">
         <v>15</v>
       </c>
       <c r="AC12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD12" t="s">
         <v>56</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>57</v>
       </c>
       <c r="AE12" t="s">
         <v>15</v>
@@ -2093,15 +2093,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13">
         <v>150</v>
@@ -2128,7 +2128,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M13" t="s">
         <v>33</v>
@@ -2152,37 +2152,37 @@
         <v>14</v>
       </c>
       <c r="T13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U13" t="s">
         <v>15</v>
       </c>
       <c r="V13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="X13" t="s">
         <v>15</v>
       </c>
       <c r="Y13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB13" t="s">
         <v>15</v>
       </c>
       <c r="AC13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD13" t="s">
         <v>56</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>57</v>
       </c>
       <c r="AE13" t="s">
         <v>15</v>
@@ -2194,15 +2194,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14">
         <v>150</v>
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M14" t="s">
         <v>33</v>
@@ -2253,37 +2253,37 @@
         <v>14</v>
       </c>
       <c r="T14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U14" t="s">
         <v>15</v>
       </c>
       <c r="V14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="X14" t="s">
         <v>15</v>
       </c>
       <c r="Y14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AA14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB14" t="s">
         <v>15</v>
       </c>
       <c r="AC14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD14" t="s">
         <v>56</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>57</v>
       </c>
       <c r="AE14" t="s">
         <v>15</v>
@@ -2295,15 +2295,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15">
         <v>150</v>
@@ -2330,7 +2330,7 @@
         <v>5</v>
       </c>
       <c r="L15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M15" t="s">
         <v>33</v>
@@ -2363,15 +2363,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16">
         <v>75</v>
@@ -2398,7 +2398,7 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M16" t="s">
         <v>33</v>
@@ -2419,7 +2419,7 @@
         <v>28</v>
       </c>
       <c r="S16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T16" t="s">
         <v>15</v>
@@ -2431,7 +2431,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Added New Battle Content
- New Changeling/Tanuki variants
- Altered stats for existing enemies (lowered Speed)
- New Midboss Music
- Renamed music tracks
- Tutorial Battles set up
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="82">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Ijiraq</t>
   </si>
   <si>
-    <t>spr_bt_ijiraq_placeholder</t>
-  </si>
-  <si>
     <t>Ijiraq2</t>
   </si>
   <si>
@@ -247,6 +244,27 @@
   </si>
   <si>
     <t>spr_bt_changeling</t>
+  </si>
+  <si>
+    <t>selfcare</t>
+  </si>
+  <si>
+    <t>spr_bt_changeling_healer</t>
+  </si>
+  <si>
+    <t>Wechselbalg</t>
+  </si>
+  <si>
+    <t>Bunbuku</t>
+  </si>
+  <si>
+    <t>spr_bt_tanuki_fire</t>
+  </si>
+  <si>
+    <t>spr_bt_ijiraq</t>
+  </si>
+  <si>
+    <t>stress</t>
   </si>
 </sst>
 </file>
@@ -1087,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG17"/>
+  <dimension ref="A1:AG19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,10 +1177,10 @@
         <v>6</v>
       </c>
       <c r="O1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q1" t="s">
         <v>22</v>
@@ -1257,7 +1275,7 @@
         <v>15</v>
       </c>
       <c r="V2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W2" t="s">
         <v>15</v>
@@ -1346,10 +1364,10 @@
         <v>15</v>
       </c>
       <c r="V3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X3" t="s">
         <v>15</v>
@@ -1426,7 +1444,7 @@
         <v>28</v>
       </c>
       <c r="S4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T4" t="s">
         <v>15</v>
@@ -1435,7 +1453,7 @@
         <v>15</v>
       </c>
       <c r="V4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W4" t="s">
         <v>15</v>
@@ -1524,10 +1542,10 @@
         <v>15</v>
       </c>
       <c r="V5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X5" t="s">
         <v>15</v>
@@ -1553,10 +1571,10 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -1618,22 +1636,22 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1642,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0.75</v>
+        <v>3</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1657,22 +1675,22 @@
         <v>33</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
         <v>2</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
       </c>
       <c r="R7" t="s">
         <v>28</v>
       </c>
       <c r="S7" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="T7" t="s">
         <v>15</v>
@@ -1686,7 +1704,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>43</v>
@@ -1701,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1710,13 +1728,13 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="L8" t="s">
         <v>31</v>
@@ -1740,7 +1758,7 @@
         <v>28</v>
       </c>
       <c r="S8" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="T8" t="s">
         <v>15</v>
@@ -1749,30 +1767,21 @@
         <v>15</v>
       </c>
       <c r="V8" t="s">
-        <v>63</v>
-      </c>
-      <c r="W8" t="s">
-        <v>15</v>
-      </c>
-      <c r="X8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D9">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1781,19 +1790,19 @@
         <v>2</v>
       </c>
       <c r="G9">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L9" t="s">
         <v>31</v>
@@ -1802,13 +1811,13 @@
         <v>33</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
+        <v>0.5</v>
+      </c>
+      <c r="P9">
         <v>2</v>
-      </c>
-      <c r="P9">
-        <v>-1</v>
       </c>
       <c r="Q9">
         <v>1</v>
@@ -1826,10 +1835,10 @@
         <v>15</v>
       </c>
       <c r="V9" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="W9" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="X9" t="s">
         <v>15</v>
@@ -1840,16 +1849,16 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D10">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1858,19 +1867,19 @@
         <v>2</v>
       </c>
       <c r="G10">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L10" t="s">
         <v>31</v>
@@ -1879,13 +1888,13 @@
         <v>33</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
+        <v>-1</v>
+      </c>
+      <c r="P10">
         <v>2</v>
-      </c>
-      <c r="P10">
-        <v>-1</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -1894,10 +1903,10 @@
         <v>28</v>
       </c>
       <c r="S10" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="T10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="U10" t="s">
         <v>15</v>
@@ -1906,7 +1915,7 @@
         <v>14</v>
       </c>
       <c r="W10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="X10" t="s">
         <v>15</v>
@@ -1917,16 +1926,16 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1935,13 +1944,13 @@
         <v>2</v>
       </c>
       <c r="G11">
-        <v>0.75</v>
+        <v>1.2</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1959,7 +1968,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>1.1000000000000001</v>
+        <v>2</v>
       </c>
       <c r="P11">
         <v>-1</v>
@@ -1971,10 +1980,10 @@
         <v>28</v>
       </c>
       <c r="S11" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="T11" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="U11" t="s">
         <v>15</v>
@@ -1983,7 +1992,7 @@
         <v>14</v>
       </c>
       <c r="W11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X11" t="s">
         <v>15</v>
@@ -1994,31 +2003,31 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D12">
-        <v>150</v>
+        <v>65</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -2027,13 +2036,13 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="M12" t="s">
         <v>33</v>
       </c>
       <c r="N12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <v>2</v>
@@ -2042,69 +2051,45 @@
         <v>-1</v>
       </c>
       <c r="Q12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R12" t="s">
         <v>28</v>
       </c>
       <c r="S12" t="s">
+        <v>62</v>
+      </c>
+      <c r="T12" t="s">
+        <v>68</v>
+      </c>
+      <c r="U12" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12" t="s">
         <v>14</v>
       </c>
-      <c r="T12" t="s">
-        <v>69</v>
-      </c>
-      <c r="U12" t="s">
-        <v>15</v>
-      </c>
-      <c r="V12" t="s">
-        <v>63</v>
-      </c>
       <c r="W12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X12" t="s">
         <v>15</v>
       </c>
       <c r="Y12" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2113,13 +2098,13 @@
         <v>2</v>
       </c>
       <c r="G13">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -2128,81 +2113,57 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="M13" t="s">
         <v>33</v>
       </c>
       <c r="N13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>0.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P13">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="Q13">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R13" t="s">
         <v>28</v>
       </c>
       <c r="S13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" t="s">
+        <v>68</v>
+      </c>
+      <c r="U13" t="s">
+        <v>15</v>
+      </c>
+      <c r="V13" t="s">
         <v>14</v>
       </c>
-      <c r="T13" t="s">
-        <v>70</v>
-      </c>
-      <c r="U13" t="s">
-        <v>15</v>
-      </c>
-      <c r="V13" t="s">
-        <v>63</v>
-      </c>
       <c r="W13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="X13" t="s">
         <v>15</v>
       </c>
       <c r="Y13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14">
         <v>150</v>
@@ -2211,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>1.5</v>
@@ -2229,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M14" t="s">
         <v>33</v>
@@ -2238,13 +2199,13 @@
         <v>0.5</v>
       </c>
       <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
         <v>-1</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>0.5</v>
-      </c>
-      <c r="Q14">
-        <v>2</v>
       </c>
       <c r="R14" t="s">
         <v>28</v>
@@ -2253,37 +2214,37 @@
         <v>14</v>
       </c>
       <c r="T14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="U14" t="s">
         <v>15</v>
       </c>
       <c r="V14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="X14" t="s">
         <v>15</v>
       </c>
       <c r="Y14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Z14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AA14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AB14" t="s">
         <v>15</v>
       </c>
       <c r="AC14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD14" t="s">
         <v>55</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>56</v>
       </c>
       <c r="AE14" t="s">
         <v>15</v>
@@ -2297,13 +2258,13 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15">
         <v>150</v>
@@ -2312,40 +2273,40 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15">
         <v>1.5</v>
       </c>
       <c r="H15">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M15" t="s">
         <v>33</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R15" t="s">
         <v>28</v>
@@ -2354,27 +2315,60 @@
         <v>14</v>
       </c>
       <c r="T15" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="U15" t="s">
         <v>15</v>
       </c>
       <c r="V15" t="s">
+        <v>62</v>
+      </c>
+      <c r="W15" t="s">
+        <v>69</v>
+      </c>
+      <c r="X15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2383,13 +2377,13 @@
         <v>2</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -2398,41 +2392,210 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M16" t="s">
         <v>33</v>
       </c>
       <c r="N16">
+        <v>0.5</v>
+      </c>
+      <c r="O16">
+        <v>-1</v>
+      </c>
+      <c r="P16">
+        <v>0.5</v>
+      </c>
+      <c r="Q16">
         <v>2</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
       </c>
       <c r="R16" t="s">
         <v>28</v>
       </c>
       <c r="S16" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="T16" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="U16" t="s">
         <v>15</v>
       </c>
       <c r="V16" t="s">
+        <v>62</v>
+      </c>
+      <c r="W16" t="s">
+        <v>66</v>
+      </c>
+      <c r="X16" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17">
+        <v>150</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>1.5</v>
+      </c>
+      <c r="H17">
+        <v>0.25</v>
+      </c>
+      <c r="I17">
+        <v>0.95</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+      <c r="L17" t="s">
+        <v>56</v>
+      </c>
+      <c r="M17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>28</v>
+      </c>
+      <c r="S17" t="s">
+        <v>14</v>
+      </c>
+      <c r="T17" t="s">
+        <v>15</v>
+      </c>
+      <c r="U17" t="s">
+        <v>15</v>
+      </c>
+      <c r="V17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18">
+        <v>75</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>56</v>
+      </c>
+      <c r="M18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18" t="s">
+        <v>28</v>
+      </c>
+      <c r="S18" t="s">
+        <v>64</v>
+      </c>
+      <c r="T18" t="s">
+        <v>15</v>
+      </c>
+      <c r="U18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tutorial Battle Scenes Mostly In
- barring tutorialization of prefixes
- includes new audio
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hughe\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D40A570A-6DAA-4B0A-B6E4-2A944C71B6C8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enemyDatabase" sheetId="1" r:id="rId1"/>
@@ -270,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1104,11 +1105,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,7 +1646,7 @@
         <v>70</v>
       </c>
       <c r="D7">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1657,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="I7">
         <v>3</v>
@@ -1858,7 +1859,7 @@
         <v>40</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1873,10 +1874,10 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="J10">
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="K10">
         <v>15</v>
@@ -1891,7 +1892,7 @@
         <v>1</v>
       </c>
       <c r="O10">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="P10">
         <v>2</v>
@@ -1906,7 +1907,7 @@
         <v>81</v>
       </c>
       <c r="T10" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="U10" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Finished Tutorial Battles + Added Dash Pop-up
- the tutorial's basically done, with edits needed
- the game yells at you for pressing the dash key now
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hughe\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D40A570A-6DAA-4B0A-B6E4-2A944C71B6C8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26ACD7A1-44EE-4EA0-B41C-6CF2DFA6B562}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1109,7 +1109,7 @@
   <dimension ref="A1:AG19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,7 +1880,7 @@
         <v>1.5</v>
       </c>
       <c r="K10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L10" t="s">
         <v>31</v>
@@ -1895,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -1936,13 +1936,13 @@
         <v>71</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>1.2</v>
@@ -1951,7 +1951,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1990,10 +1990,10 @@
         <v>15</v>
       </c>
       <c r="V11" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="W11" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="X11" t="s">
         <v>15</v>
@@ -2013,7 +2013,7 @@
         <v>71</v>
       </c>
       <c r="D12">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2022,13 +2022,13 @@
         <v>2</v>
       </c>
       <c r="G12">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -2046,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P12">
         <v>-1</v>

</xml_diff>

<commit_message>
Added ala, kitsunario/uigi, and tanuki variants, made slugcon wave layout
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hughe\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD0BAFE-0401-489B-B643-B03860F4C1DC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB0A1BE4-FC5A-4B9C-9159-72B7330B3F72}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enemyDatabase" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="92">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -272,6 +272,30 @@
   </si>
   <si>
     <t>wech_1</t>
+  </si>
+  <si>
+    <t>Ala</t>
+  </si>
+  <si>
+    <t>spr_bt_ala</t>
+  </si>
+  <si>
+    <t>Kitsunario</t>
+  </si>
+  <si>
+    <t>Kitsunuigi</t>
+  </si>
+  <si>
+    <t>Tanooki</t>
+  </si>
+  <si>
+    <t>Tater Totnuki</t>
+  </si>
+  <si>
+    <t>spr_bt_kitsune</t>
+  </si>
+  <si>
+    <t>spr_bt_kitsune_mountain_dew</t>
   </si>
 </sst>
 </file>
@@ -1112,35 +1136,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG19"/>
+  <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="3" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="3" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" customWidth="1"/>
-    <col min="25" max="25" width="19.140625" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" customWidth="1"/>
+    <col min="25" max="25" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1217,7 +1241,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1306,7 +1330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1395,7 +1419,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1484,7 +1508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1573,7 +1597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1641,7 +1665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -1658,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1709,7 +1733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1777,7 +1801,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1854,7 +1878,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -1931,18 +1955,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1951,13 +1975,13 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1972,13 +1996,13 @@
         <v>33</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
+        <v>0.5</v>
+      </c>
+      <c r="P11">
         <v>2</v>
-      </c>
-      <c r="P11">
-        <v>-1</v>
       </c>
       <c r="Q11">
         <v>1</v>
@@ -1987,7 +2011,7 @@
         <v>28</v>
       </c>
       <c r="S11" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="T11" t="s">
         <v>15</v>
@@ -1996,45 +2020,36 @@
         <v>15</v>
       </c>
       <c r="V11" t="s">
-        <v>58</v>
-      </c>
-      <c r="W11" t="s">
-        <v>15</v>
-      </c>
-      <c r="X11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="D12">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -2049,13 +2064,13 @@
         <v>33</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="P12">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Q12">
         <v>1</v>
@@ -2067,27 +2082,18 @@
         <v>58</v>
       </c>
       <c r="T12" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="U12" t="s">
         <v>15</v>
       </c>
       <c r="V12" t="s">
-        <v>14</v>
-      </c>
-      <c r="W12" t="s">
-        <v>64</v>
-      </c>
-      <c r="X12" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
@@ -2096,22 +2102,22 @@
         <v>67</v>
       </c>
       <c r="D13">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0.75</v>
+        <v>1.2</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -2129,7 +2135,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>1.1000000000000001</v>
+        <v>2</v>
       </c>
       <c r="P13">
         <v>-1</v>
@@ -2141,19 +2147,19 @@
         <v>28</v>
       </c>
       <c r="S13" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="T13" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="U13" t="s">
         <v>15</v>
       </c>
       <c r="V13" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="W13" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="X13" t="s">
         <v>15</v>
@@ -2162,33 +2168,33 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14">
-        <v>1.25</v>
+        <v>1.3</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -2197,28 +2203,28 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="M14" t="s">
         <v>33</v>
       </c>
       <c r="N14">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P14">
         <v>-1</v>
       </c>
       <c r="Q14">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R14" t="s">
         <v>28</v>
       </c>
       <c r="S14" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="T14" t="s">
         <v>64</v>
@@ -2227,7 +2233,7 @@
         <v>15</v>
       </c>
       <c r="V14" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="W14" t="s">
         <v>64</v>
@@ -2236,45 +2242,21 @@
         <v>15</v>
       </c>
       <c r="Y14" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15">
-        <v>170</v>
+        <v>45</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2283,13 +2265,13 @@
         <v>2</v>
       </c>
       <c r="G15">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -2298,99 +2280,75 @@
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="M15" t="s">
         <v>33</v>
       </c>
       <c r="N15">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>0.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P15">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="Q15">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R15" t="s">
         <v>28</v>
       </c>
       <c r="S15" t="s">
+        <v>59</v>
+      </c>
+      <c r="T15" t="s">
+        <v>64</v>
+      </c>
+      <c r="U15" t="s">
+        <v>15</v>
+      </c>
+      <c r="V15" t="s">
         <v>14</v>
       </c>
-      <c r="T15" t="s">
-        <v>65</v>
-      </c>
-      <c r="U15" t="s">
-        <v>15</v>
-      </c>
-      <c r="V15" t="s">
-        <v>58</v>
-      </c>
       <c r="W15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="X15" t="s">
         <v>15</v>
       </c>
       <c r="Y15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D16">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -2399,19 +2357,19 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="M16" t="s">
         <v>33</v>
       </c>
       <c r="N16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O16">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="P16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q16">
         <v>2</v>
@@ -2423,99 +2381,66 @@
         <v>14</v>
       </c>
       <c r="T16" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="U16" t="s">
         <v>15</v>
       </c>
       <c r="V16" t="s">
-        <v>58</v>
-      </c>
-      <c r="W16" t="s">
-        <v>62</v>
-      </c>
-      <c r="X16" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D17">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="J17">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="M17" t="s">
         <v>33</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R17" t="s">
         <v>28</v>
@@ -2533,33 +2458,33 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D18">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -2568,28 +2493,28 @@
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="M18" t="s">
         <v>33</v>
       </c>
       <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
         <v>2</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
       </c>
       <c r="R18" t="s">
         <v>28</v>
       </c>
       <c r="S18" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="T18" t="s">
         <v>15</v>
@@ -2601,8 +2526,447 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19">
+        <v>170</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1.25</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0.8</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M19" t="s">
+        <v>33</v>
+      </c>
+      <c r="N19">
+        <v>0.5</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>-1</v>
+      </c>
+      <c r="Q19">
+        <v>0.5</v>
+      </c>
+      <c r="R19" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" t="s">
+        <v>14</v>
+      </c>
+      <c r="T19" t="s">
+        <v>64</v>
+      </c>
+      <c r="U19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" t="s">
+        <v>58</v>
+      </c>
+      <c r="W19" t="s">
+        <v>64</v>
+      </c>
+      <c r="X19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20">
+        <v>170</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>1.25</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0.8</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>52</v>
+      </c>
+      <c r="M20" t="s">
+        <v>33</v>
+      </c>
+      <c r="N20">
+        <v>0.5</v>
+      </c>
+      <c r="O20">
+        <v>0.5</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>-1</v>
+      </c>
+      <c r="R20" t="s">
+        <v>28</v>
+      </c>
+      <c r="S20" t="s">
+        <v>14</v>
+      </c>
+      <c r="T20" t="s">
+        <v>65</v>
+      </c>
+      <c r="U20" t="s">
+        <v>15</v>
+      </c>
+      <c r="V20" t="s">
+        <v>58</v>
+      </c>
+      <c r="W20" t="s">
+        <v>65</v>
+      </c>
+      <c r="X20" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21">
+        <v>170</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>1.25</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0.8</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>52</v>
+      </c>
+      <c r="M21" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21">
+        <v>0.5</v>
+      </c>
+      <c r="O21">
+        <v>-1</v>
+      </c>
+      <c r="P21">
+        <v>0.5</v>
+      </c>
+      <c r="Q21">
+        <v>2</v>
+      </c>
+      <c r="R21" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21" t="s">
+        <v>14</v>
+      </c>
+      <c r="T21" t="s">
+        <v>62</v>
+      </c>
+      <c r="U21" t="s">
+        <v>15</v>
+      </c>
+      <c r="V21" t="s">
+        <v>58</v>
+      </c>
+      <c r="W21" t="s">
+        <v>62</v>
+      </c>
+      <c r="X21" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22">
+        <v>170</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>0.75</v>
+      </c>
+      <c r="H22">
+        <v>0.25</v>
+      </c>
+      <c r="I22">
+        <v>1.2</v>
+      </c>
+      <c r="J22">
+        <v>0.9</v>
+      </c>
+      <c r="K22">
+        <v>5</v>
+      </c>
+      <c r="L22" t="s">
+        <v>52</v>
+      </c>
+      <c r="M22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22" t="s">
+        <v>28</v>
+      </c>
+      <c r="S22" t="s">
+        <v>14</v>
+      </c>
+      <c r="T22" t="s">
+        <v>15</v>
+      </c>
+      <c r="U22" t="s">
+        <v>15</v>
+      </c>
+      <c r="V22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23">
+        <v>75</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>3</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>52</v>
+      </c>
+      <c r="M23" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23" t="s">
+        <v>60</v>
+      </c>
+      <c r="T23" t="s">
+        <v>15</v>
+      </c>
+      <c r="U23" t="s">
+        <v>15</v>
+      </c>
+      <c r="V23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More Balancing, added some random spells, added Global battle events, Greatly expanded battle event capabilities
-Added the BattleEventManager class, a battle event that groups a number of other battle events into a list and checks them when its checkTrigger is called (used to implement global BEs)
-Added a BELogicTrigger, a BE that triggeres and event based on the result of an array of other BEs and a specified logical operator (OR,AND,NOR,NAND,NOT,XOR,XNOR) can be chained together (this has no use right now but it was fun)
-Expanded SPecific attack to be able to check caster, take ANY field position as target and/or caster, and to be able to specifiy any combination of keywords that must be present
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE502081-A223-466D-800C-F9FA1CED165A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215B56FA-3EBB-4238-BCB2-B92C4927DAFD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1679,7 +1679,7 @@
         <v>83</v>
       </c>
       <c r="D7">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1712,13 +1712,13 @@
         <v>2</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P7">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="Q7">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="R7" t="s">
         <v>28</v>
@@ -1904,10 +1904,10 @@
         <v>1.3</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I10">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="J10">
         <v>1.5</v>

</xml_diff>

<commit_message>
fixed the form changing bugs
-removed the double form change
-made setting the stats from AI seperate from changing the form
-made formChange stop itself before repeating
-made formChange wait for pause to end
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215B56FA-3EBB-4238-BCB2-B92C4927DAFD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D2FC67-D20B-4683-B9EA-39122F4C3028}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1679,7 +1679,7 @@
         <v>83</v>
       </c>
       <c r="D7">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1901,7 +1901,7 @@
         <v>2</v>
       </c>
       <c r="G10">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>0.2</v>
@@ -2111,10 +2111,10 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>1.2</v>
+        <v>11</v>
       </c>
       <c r="H13">
         <v>0</v>

</xml_diff>

<commit_message>
Balanced doppel, fixed more form change issues, added sfx, added more audio channels, nerfed status effects, more
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D2FC67-D20B-4683-B9EA-39122F4C3028}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76D0936-2DAD-40AA-9FCA-F81F43CEABDB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1142,7 +1142,7 @@
   <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2579,7 +2579,7 @@
         <v>33</v>
       </c>
       <c r="N19">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="O19">
         <v>2</v>
@@ -2680,7 +2680,7 @@
         <v>33</v>
       </c>
       <c r="N20">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="O20">
         <v>0.5</v>
@@ -2781,7 +2781,7 @@
         <v>33</v>
       </c>
       <c r="N21">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="O21">
         <v>-1</v>
@@ -2867,13 +2867,13 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>0.65</v>
+        <v>0.4</v>
       </c>
       <c r="J22">
         <v>0.9</v>
       </c>
       <c r="K22">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L22" t="s">
         <v>52</v>
@@ -2882,7 +2882,7 @@
         <v>33</v>
       </c>
       <c r="N22">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="O22">
         <v>0</v>

</xml_diff>

<commit_message>
Added some spells, added kitsune, added the form change AI type
Kitsune not complete: no riddles yet, unbalanced, and their Tanuki forms don't match the stats (as the reflect problem is not solved)
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76D0936-2DAD-40AA-9FCA-F81F43CEABDB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E907DD33-7D37-4768-A42D-F7D2F4146074}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="102">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -299,6 +299,33 @@
   </si>
   <si>
     <t>35,25</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sword </t>
+  </si>
+  <si>
+    <t>GROUP/HEALTH_CRITICAL</t>
+  </si>
+  <si>
+    <t>halberd</t>
+  </si>
+  <si>
+    <t>empowered</t>
+  </si>
+  <si>
+    <t>weakened</t>
+  </si>
+  <si>
+    <t>FormChange1</t>
+  </si>
+  <si>
+    <t>HealthLow1,Kitsunario,false</t>
+  </si>
+  <si>
+    <t>HealthLow1,Kitsunuigi,false</t>
   </si>
 </sst>
 </file>
@@ -1139,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG24"/>
+  <dimension ref="A1:AM24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1151,7 +1178,7 @@
     <col min="2" max="3" width="14.5546875" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" customWidth="1"/>
     <col min="13" max="13" width="13.109375" customWidth="1"/>
     <col min="14" max="14" width="9.6640625" customWidth="1"/>
     <col min="15" max="15" width="9.88671875" customWidth="1"/>
@@ -1167,7 +1194,7 @@
     <col min="25" max="25" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1271,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1333,7 +1360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1422,7 +1449,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1511,7 +1538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1588,19 +1615,31 @@
         <v>29</v>
       </c>
       <c r="Z5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AA5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE5" t="s">
         <v>62</v>
       </c>
-      <c r="AB5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC5" t="s">
+      <c r="AF5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1668,7 +1707,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -1736,7 +1775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1804,7 +1843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1881,7 +1920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -1958,7 +1997,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -1969,13 +2008,13 @@
         <v>40</v>
       </c>
       <c r="D11">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1987,16 +2026,16 @@
         <v>0.75</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="M11" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -2014,7 +2053,7 @@
         <v>28</v>
       </c>
       <c r="S11" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="T11" t="s">
         <v>15</v>
@@ -2026,7 +2065,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -2037,13 +2076,13 @@
         <v>40</v>
       </c>
       <c r="D12">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2055,16 +2094,16 @@
         <v>0.75</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="M12" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -2094,7 +2133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -2171,7 +2210,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -2248,7 +2287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -2325,7 +2364,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -2402,7 +2441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -2419,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -2428,28 +2467,28 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L17" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="M17" t="s">
         <v>33</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="Q17">
         <v>2</v>
@@ -2461,16 +2500,67 @@
         <v>14</v>
       </c>
       <c r="T17" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="U17" t="s">
         <v>15</v>
       </c>
       <c r="V17" t="s">
+        <v>58</v>
+      </c>
+      <c r="W17" t="s">
+        <v>64</v>
+      </c>
+      <c r="X17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -2481,13 +2571,13 @@
         <v>66</v>
       </c>
       <c r="D18">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2496,31 +2586,31 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L18" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="M18" t="s">
         <v>33</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="O18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="Q18">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="R18" t="s">
         <v>28</v>
@@ -2529,16 +2619,67 @@
         <v>14</v>
       </c>
       <c r="T18" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="U18" t="s">
         <v>15</v>
       </c>
       <c r="V18" t="s">
+        <v>14</v>
+      </c>
+      <c r="W18" t="s">
+        <v>15</v>
+      </c>
+      <c r="X18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -2639,7 +2780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2740,7 +2881,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -2841,7 +2982,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -2909,7 +3050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -2977,7 +3118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
scouter not updating and reflect not updating scouter fixed
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E907DD33-7D37-4768-A42D-F7D2F4146074}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624F8D07-1AF6-494A-B679-607162C279F8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1169,7 +1169,7 @@
   <dimension ref="A1:AM24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1659,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2153,7 +2153,7 @@
         <v>2</v>
       </c>
       <c r="G13">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2384,7 +2384,7 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2461,13 +2461,13 @@
         <v>3</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="J17">
         <v>0.9</v>
@@ -2580,13 +2580,13 @@
         <v>2</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="J18">
         <v>0.9</v>

</xml_diff>

<commit_message>
Bug fixes to build
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34281DA-B40E-4A37-90DA-63BA89525AF4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECCD325-3B92-46DA-81AD-D7B0CF48452E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1169,7 +1169,7 @@
   <dimension ref="A1:AM24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2153,7 +2153,7 @@
         <v>2</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2384,7 +2384,7 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2586,7 +2586,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>7</v>
+        <v>0.7</v>
       </c>
       <c r="J18">
         <v>0.9</v>

</xml_diff>

<commit_message>
Updated Typocrypha/Player HP Display, Popups
- Typocrypha HP bar is now up to date
- Some changes to element pop-ups have started
- K.O./Overkill popups replaced with Critical
- Added the enemy "Adderstone"
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hughe\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECCD325-3B92-46DA-81AD-D7B0CF48452E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6B11559-DCCD-468C-B422-C945820CB4DA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enemyDatabase" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="104">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -326,6 +326,12 @@
   </si>
   <si>
     <t>HealthLow1,Kitsunuigi,false</t>
+  </si>
+  <si>
+    <t>Adderstone</t>
+  </si>
+  <si>
+    <t>spr_bt_adderstone</t>
   </si>
 </sst>
 </file>
@@ -1166,35 +1172,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM24"/>
+  <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="3" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" customWidth="1"/>
-    <col min="18" max="18" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="3" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="11.5546875" customWidth="1"/>
-    <col min="21" max="21" width="10.33203125" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="11.33203125" customWidth="1"/>
-    <col min="25" max="25" width="19.109375" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" customWidth="1"/>
+    <col min="25" max="25" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1271,7 +1277,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1360,7 +1366,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1449,7 +1455,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1639,7 +1645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1707,7 +1713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1920,7 +1926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -1997,7 +2003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -2065,7 +2071,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -2287,7 +2293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -2364,7 +2370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -2441,15 +2447,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="D17">
         <v>100</v>
@@ -2461,34 +2467,34 @@
         <v>3</v>
       </c>
       <c r="G17">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="J17">
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="K17">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="M17" t="s">
         <v>33</v>
       </c>
       <c r="N17">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="O17">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="P17">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="Q17">
         <v>2</v>
@@ -2500,84 +2506,54 @@
         <v>14</v>
       </c>
       <c r="T17" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="U17" t="s">
         <v>15</v>
       </c>
       <c r="V17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="W17" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="X17" t="s">
         <v>15</v>
       </c>
       <c r="Y17" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="Z17" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="AA17" t="s">
         <v>15</v>
       </c>
       <c r="AB17" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="AC17" t="s">
-        <v>96</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>95</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
         <v>66</v>
       </c>
       <c r="D18">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18">
         <v>0.75</v>
@@ -2604,13 +2580,13 @@
         <v>-2</v>
       </c>
       <c r="O18">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="P18">
         <v>-2</v>
       </c>
       <c r="Q18">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="R18" t="s">
         <v>28</v>
@@ -2619,25 +2595,25 @@
         <v>14</v>
       </c>
       <c r="T18" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="U18" t="s">
         <v>15</v>
       </c>
       <c r="V18" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="W18" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="X18" t="s">
         <v>15</v>
       </c>
       <c r="Y18" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="Z18" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="AA18" t="s">
         <v>15</v>
@@ -2646,13 +2622,13 @@
         <v>29</v>
       </c>
       <c r="AC18" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="AD18" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="AE18" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AF18" t="s">
         <v>14</v>
@@ -2667,54 +2643,54 @@
         <v>95</v>
       </c>
       <c r="AJ18" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="AK18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AL18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AM18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D19">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="M19" t="s">
         <v>33</v>
@@ -2726,10 +2702,10 @@
         <v>2</v>
       </c>
       <c r="P19">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="Q19">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="R19" t="s">
         <v>28</v>
@@ -2738,54 +2714,72 @@
         <v>14</v>
       </c>
       <c r="T19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" t="s">
+        <v>14</v>
+      </c>
+      <c r="W19" t="s">
+        <v>15</v>
+      </c>
+      <c r="X19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK19" t="s">
         <v>64</v>
       </c>
-      <c r="U19" t="s">
-        <v>15</v>
-      </c>
-      <c r="V19" t="s">
-        <v>58</v>
-      </c>
-      <c r="W19" t="s">
-        <v>64</v>
-      </c>
-      <c r="X19" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG19" t="s">
+      <c r="AL19" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
         <v>68</v>
@@ -2797,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>1.25</v>
@@ -2824,13 +2818,13 @@
         <v>-2</v>
       </c>
       <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>-1</v>
+      </c>
+      <c r="Q20">
         <v>0.5</v>
-      </c>
-      <c r="P20">
-        <v>2</v>
-      </c>
-      <c r="Q20">
-        <v>-1</v>
       </c>
       <c r="R20" t="s">
         <v>28</v>
@@ -2839,7 +2833,7 @@
         <v>14</v>
       </c>
       <c r="T20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U20" t="s">
         <v>15</v>
@@ -2848,7 +2842,7 @@
         <v>58</v>
       </c>
       <c r="W20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="X20" t="s">
         <v>15</v>
@@ -2860,7 +2854,7 @@
         <v>60</v>
       </c>
       <c r="AA20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB20" t="s">
         <v>15</v>
@@ -2881,12 +2875,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
         <v>68</v>
@@ -2925,13 +2919,13 @@
         <v>-2</v>
       </c>
       <c r="O21">
+        <v>0.5</v>
+      </c>
+      <c r="P21">
+        <v>2</v>
+      </c>
+      <c r="Q21">
         <v>-1</v>
-      </c>
-      <c r="P21">
-        <v>0.5</v>
-      </c>
-      <c r="Q21">
-        <v>2</v>
       </c>
       <c r="R21" t="s">
         <v>28</v>
@@ -2940,7 +2934,7 @@
         <v>14</v>
       </c>
       <c r="T21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="U21" t="s">
         <v>15</v>
@@ -2949,7 +2943,7 @@
         <v>58</v>
       </c>
       <c r="W21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="X21" t="s">
         <v>15</v>
@@ -2961,7 +2955,7 @@
         <v>60</v>
       </c>
       <c r="AA21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AB21" t="s">
         <v>15</v>
@@ -2982,12 +2976,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
         <v>68</v>
@@ -2999,19 +2993,19 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="J22">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -3026,13 +3020,13 @@
         <v>-2</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R22" t="s">
         <v>28</v>
@@ -3041,45 +3035,78 @@
         <v>14</v>
       </c>
       <c r="T22" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="U22" t="s">
         <v>15</v>
       </c>
       <c r="V22" t="s">
+        <v>58</v>
+      </c>
+      <c r="W22" t="s">
+        <v>62</v>
+      </c>
+      <c r="X22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
         <v>68</v>
       </c>
       <c r="D23">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -3091,7 +3118,7 @@
         <v>33</v>
       </c>
       <c r="N23">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -3106,7 +3133,7 @@
         <v>28</v>
       </c>
       <c r="S23" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="T23" t="s">
         <v>15</v>
@@ -3118,8 +3145,76 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24">
+        <v>75</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>52</v>
+      </c>
+      <c r="M24" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24" t="s">
+        <v>28</v>
+      </c>
+      <c r="S24" t="s">
+        <v>60</v>
+      </c>
+      <c r="T24" t="s">
+        <v>15</v>
+      </c>
+      <c r="U24" t="s">
+        <v>15</v>
+      </c>
+      <c r="V24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bloacked out all battles and interrupts, added cat macroes, added self and other keywords, implemented some scenes and interrupts
-not fully tested yet
-Illyia and Dahlia are unkillable (no transforms so far, but planning on adding one)
-also added example dialogue for setting info
-
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hughe\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47247012-1D3E-41BE-B99F-FE779975CAED}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AACCA9-9EF9-485B-82CD-7C988D3BDBE7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enemyDatabase" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="117">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -356,6 +356,21 @@
   </si>
   <si>
     <t>debilitate</t>
+  </si>
+  <si>
+    <t>Doppelganger</t>
+  </si>
+  <si>
+    <t>Attacker1,Bunbuku,true</t>
+  </si>
+  <si>
+    <t>Illyia?</t>
+  </si>
+  <si>
+    <t>Dahlia?</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -1196,35 +1211,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM26"/>
+  <dimension ref="A1:AM29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="3" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="3" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" customWidth="1"/>
     <col min="23" max="23" width="10" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" customWidth="1"/>
-    <col min="25" max="25" width="19.140625" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" customWidth="1"/>
+    <col min="25" max="25" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1316,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1390,7 +1405,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1479,7 +1494,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1568,7 +1583,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1669,7 +1684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1737,7 +1752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -1805,7 +1820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1873,7 +1888,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1950,7 +1965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -2027,7 +2042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -2095,7 +2110,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -2163,7 +2178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -2240,7 +2255,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -2317,7 +2332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -2394,7 +2409,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -2471,7 +2486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -2560,7 +2575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>104</v>
       </c>
@@ -2667,7 +2682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -2786,7 +2801,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -2905,33 +2920,33 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
         <v>68</v>
       </c>
       <c r="D21">
-        <v>170</v>
+        <v>300</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G21">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I21">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -2940,19 +2955,19 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="M21" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="N21">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="O21">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P21">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="Q21">
         <v>0.5</v>
@@ -2964,7 +2979,7 @@
         <v>14</v>
       </c>
       <c r="T21" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="U21" t="s">
         <v>15</v>
@@ -2973,51 +2988,27 @@
         <v>58</v>
       </c>
       <c r="W21" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="X21" t="s">
         <v>15</v>
       </c>
       <c r="Y21" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D22">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -3026,13 +3017,13 @@
         <v>2</v>
       </c>
       <c r="G22">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -3041,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="L22" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="M22" t="s">
         <v>33</v>
@@ -3050,75 +3041,60 @@
         <v>-2</v>
       </c>
       <c r="O22">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="P22">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="Q22">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="R22" t="s">
         <v>28</v>
       </c>
       <c r="S22" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="T22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U22" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="V22" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="W22" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="X22" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="Y22" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="Z22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AA22" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="AB22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D23">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -3127,13 +3103,13 @@
         <v>2</v>
       </c>
       <c r="G23">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -3142,7 +3118,7 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="M23" t="s">
         <v>33</v>
@@ -3151,66 +3127,51 @@
         <v>-2</v>
       </c>
       <c r="O23">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="P23">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="Q23">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="R23" t="s">
         <v>28</v>
       </c>
       <c r="S23" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="T23" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="U23" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="V23" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="W23" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="X23" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="Y23" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="Z23" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="AA23" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="AB23" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE23" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF23" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
         <v>78</v>
@@ -3225,19 +3186,19 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="J24">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -3252,13 +3213,13 @@
         <v>-2</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R24" t="s">
         <v>28</v>
@@ -3267,27 +3228,60 @@
         <v>14</v>
       </c>
       <c r="T24" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="U24" t="s">
         <v>15</v>
       </c>
       <c r="V24" t="s">
+        <v>58</v>
+      </c>
+      <c r="W24" t="s">
+        <v>64</v>
+      </c>
+      <c r="X24" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
         <v>68</v>
       </c>
       <c r="D25">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -3296,13 +3290,13 @@
         <v>2</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -3317,35 +3311,305 @@
         <v>33</v>
       </c>
       <c r="N25">
+        <v>-2</v>
+      </c>
+      <c r="O25">
+        <v>0.5</v>
+      </c>
+      <c r="P25">
         <v>2</v>
       </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
       <c r="Q25">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R25" t="s">
         <v>28</v>
       </c>
       <c r="S25" t="s">
+        <v>14</v>
+      </c>
+      <c r="T25" t="s">
+        <v>65</v>
+      </c>
+      <c r="U25" t="s">
+        <v>15</v>
+      </c>
+      <c r="V25" t="s">
+        <v>58</v>
+      </c>
+      <c r="W25" t="s">
+        <v>65</v>
+      </c>
+      <c r="X25" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z25" t="s">
         <v>60</v>
       </c>
-      <c r="T25" t="s">
-        <v>15</v>
-      </c>
-      <c r="U25" t="s">
-        <v>15</v>
-      </c>
-      <c r="V25" t="s">
+      <c r="AA25" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26">
+        <v>170</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>1.25</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0.8</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>52</v>
+      </c>
+      <c r="M26" t="s">
+        <v>33</v>
+      </c>
+      <c r="N26">
+        <v>-2</v>
+      </c>
+      <c r="O26">
+        <v>-1</v>
+      </c>
+      <c r="P26">
+        <v>0.5</v>
+      </c>
+      <c r="Q26">
+        <v>2</v>
+      </c>
+      <c r="R26" t="s">
+        <v>28</v>
+      </c>
+      <c r="S26" t="s">
+        <v>14</v>
+      </c>
+      <c r="T26" t="s">
+        <v>62</v>
+      </c>
+      <c r="U26" t="s">
+        <v>15</v>
+      </c>
+      <c r="V26" t="s">
+        <v>58</v>
+      </c>
+      <c r="W26" t="s">
+        <v>62</v>
+      </c>
+      <c r="X26" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27">
+        <v>170</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>1.5</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0.4</v>
+      </c>
+      <c r="J27">
+        <v>0.9</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
+        <v>52</v>
+      </c>
+      <c r="M27" t="s">
+        <v>33</v>
+      </c>
+      <c r="N27">
+        <v>-2</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27" t="s">
+        <v>28</v>
+      </c>
+      <c r="S27" t="s">
+        <v>14</v>
+      </c>
+      <c r="T27" t="s">
+        <v>15</v>
+      </c>
+      <c r="U27" t="s">
+        <v>15</v>
+      </c>
+      <c r="V27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28">
+        <v>75</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>52</v>
+      </c>
+      <c r="M28" t="s">
+        <v>33</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28" t="s">
+        <v>28</v>
+      </c>
+      <c r="S28" t="s">
+        <v>60</v>
+      </c>
+      <c r="T28" t="s">
+        <v>15</v>
+      </c>
+      <c r="U28" t="s">
+        <v>15</v>
+      </c>
+      <c r="V28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added form changing mechanics for I/D doppels, swapped some sprites out, did preliminary balancing, revamped target mods, added some new target mods, added some new spells
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AACCA9-9EF9-485B-82CD-7C988D3BDBE7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3A5FE1-30D9-4E83-B072-04F263CB4FF1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="125">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -178,9 +178,6 @@
     <t>magic_circle</t>
   </si>
   <si>
-    <t>Doppleganger1</t>
-  </si>
-  <si>
     <t>Doppelganger (BLUE)</t>
   </si>
   <si>
@@ -371,6 +368,33 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>spr_bt_doppelganger_illyia</t>
+  </si>
+  <si>
+    <t>spr_bt_doppelganger_dahlia</t>
+  </si>
+  <si>
+    <t>spr_bt_illyia</t>
+  </si>
+  <si>
+    <t>spr_bt_dahlia</t>
+  </si>
+  <si>
+    <t>Doppelganger1</t>
+  </si>
+  <si>
+    <t>DoppelFriend1</t>
+  </si>
+  <si>
+    <t>Illyia???</t>
+  </si>
+  <si>
+    <t>Dahlia???</t>
+  </si>
+  <si>
+    <t>widened</t>
   </si>
 </sst>
 </file>
@@ -513,7 +537,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,6 +717,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -854,8 +884,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1211,10 +1242,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM29"/>
+  <dimension ref="A1:AM31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,80 +1273,80 @@
     <col min="25" max="25" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:33" s="1" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1381,7 +1415,7 @@
         <v>15</v>
       </c>
       <c r="V2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W2" t="s">
         <v>15</v>
@@ -1443,7 +1477,7 @@
         <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N3">
         <v>-1</v>
@@ -1470,10 +1504,10 @@
         <v>15</v>
       </c>
       <c r="V3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X3" t="s">
         <v>15</v>
@@ -1526,7 +1560,7 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L4" t="s">
         <v>31</v>
@@ -1550,7 +1584,7 @@
         <v>28</v>
       </c>
       <c r="S4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T4" t="s">
         <v>15</v>
@@ -1559,7 +1593,7 @@
         <v>15</v>
       </c>
       <c r="V4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W4" t="s">
         <v>15</v>
@@ -1571,7 +1605,7 @@
         <v>29</v>
       </c>
       <c r="Z4" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="AA4" t="s">
         <v>15</v>
@@ -1639,10 +1673,10 @@
         <v>28</v>
       </c>
       <c r="S5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U5" t="s">
         <v>15</v>
@@ -1651,7 +1685,7 @@
         <v>14</v>
       </c>
       <c r="W5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="X5" t="s">
         <v>15</v>
@@ -1660,22 +1694,22 @@
         <v>29</v>
       </c>
       <c r="Z5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB5" t="s">
         <v>15</v>
       </c>
       <c r="AC5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AD5" t="s">
         <v>14</v>
       </c>
       <c r="AE5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AF5" t="s">
         <v>15</v>
@@ -1689,10 +1723,10 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6">
         <v>18</v>
@@ -1754,13 +1788,13 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7">
         <v>90</v>
@@ -1796,19 +1830,19 @@
         <v>2</v>
       </c>
       <c r="O7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R7" t="s">
         <v>28</v>
       </c>
       <c r="S7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T7" t="s">
         <v>15</v>
@@ -1876,7 +1910,7 @@
         <v>28</v>
       </c>
       <c r="S8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T8" t="s">
         <v>15</v>
@@ -1953,7 +1987,7 @@
         <v>15</v>
       </c>
       <c r="V9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W9" t="s">
         <v>15</v>
@@ -1967,13 +2001,13 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -2021,7 +2055,7 @@
         <v>28</v>
       </c>
       <c r="S10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T10" t="s">
         <v>15</v>
@@ -2033,7 +2067,7 @@
         <v>14</v>
       </c>
       <c r="W10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X10" t="s">
         <v>15</v>
@@ -2044,7 +2078,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
@@ -2077,10 +2111,10 @@
         <v>10</v>
       </c>
       <c r="L11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M11" t="s">
         <v>99</v>
-      </c>
-      <c r="M11" t="s">
-        <v>100</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -2112,7 +2146,7 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
@@ -2145,10 +2179,10 @@
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -2166,7 +2200,7 @@
         <v>28</v>
       </c>
       <c r="S12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T12" t="s">
         <v>15</v>
@@ -2183,10 +2217,10 @@
         <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13">
         <v>50</v>
@@ -2237,16 +2271,16 @@
         <v>14</v>
       </c>
       <c r="T13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U13" t="s">
         <v>15</v>
       </c>
       <c r="V13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X13" t="s">
         <v>15</v>
@@ -2260,10 +2294,10 @@
         <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14">
         <v>120</v>
@@ -2311,10 +2345,10 @@
         <v>28</v>
       </c>
       <c r="S14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U14" t="s">
         <v>15</v>
@@ -2323,7 +2357,7 @@
         <v>14</v>
       </c>
       <c r="W14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X14" t="s">
         <v>15</v>
@@ -2334,13 +2368,13 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15">
         <v>45</v>
@@ -2388,10 +2422,10 @@
         <v>28</v>
       </c>
       <c r="S15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U15" t="s">
         <v>15</v>
@@ -2400,7 +2434,7 @@
         <v>14</v>
       </c>
       <c r="W15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X15" t="s">
         <v>15</v>
@@ -2411,13 +2445,13 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
         <v>84</v>
       </c>
-      <c r="B16" t="s">
-        <v>85</v>
-      </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16">
         <v>65</v>
@@ -2465,19 +2499,19 @@
         <v>28</v>
       </c>
       <c r="S16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U16" t="s">
         <v>15</v>
       </c>
       <c r="V16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="X16" t="s">
         <v>15</v>
@@ -2488,10 +2522,10 @@
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
@@ -2521,10 +2555,10 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -2551,7 +2585,7 @@
         <v>15</v>
       </c>
       <c r="V17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W17" t="s">
         <v>15</v>
@@ -2577,10 +2611,10 @@
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -2631,7 +2665,7 @@
         <v>28</v>
       </c>
       <c r="S18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T18" t="s">
         <v>15</v>
@@ -2640,25 +2674,25 @@
         <v>15</v>
       </c>
       <c r="V18" t="s">
+        <v>109</v>
+      </c>
+      <c r="W18" t="s">
+        <v>61</v>
+      </c>
+      <c r="X18" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y18" t="s">
         <v>110</v>
       </c>
-      <c r="W18" t="s">
-        <v>62</v>
-      </c>
-      <c r="X18" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>111</v>
-      </c>
       <c r="Z18" t="s">
         <v>15</v>
       </c>
       <c r="AA18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC18" t="s">
         <v>15</v>
@@ -2670,7 +2704,7 @@
         <v>29</v>
       </c>
       <c r="AF18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AG18" t="s">
         <v>15</v>
@@ -2684,13 +2718,13 @@
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19">
         <v>100</v>
@@ -2717,7 +2751,7 @@
         <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M19" t="s">
         <v>33</v>
@@ -2741,22 +2775,22 @@
         <v>14</v>
       </c>
       <c r="T19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U19" t="s">
         <v>15</v>
       </c>
       <c r="V19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X19" t="s">
         <v>15</v>
       </c>
       <c r="Y19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z19" t="s">
         <v>15</v>
@@ -2768,7 +2802,7 @@
         <v>29</v>
       </c>
       <c r="AC19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AD19" t="s">
         <v>15</v>
@@ -2786,16 +2820,16 @@
         <v>15</v>
       </c>
       <c r="AI19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AJ19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AK19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AL19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AM19" t="s">
         <v>16</v>
@@ -2803,13 +2837,13 @@
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20">
         <v>150</v>
@@ -2836,7 +2870,7 @@
         <v>10</v>
       </c>
       <c r="L20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M20" t="s">
         <v>33</v>
@@ -2860,7 +2894,7 @@
         <v>14</v>
       </c>
       <c r="T20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U20" t="s">
         <v>15</v>
@@ -2875,10 +2909,10 @@
         <v>15</v>
       </c>
       <c r="Y20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Z20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AA20" t="s">
         <v>15</v>
@@ -2887,10 +2921,10 @@
         <v>29</v>
       </c>
       <c r="AC20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AE20" t="s">
         <v>15</v>
@@ -2905,16 +2939,16 @@
         <v>15</v>
       </c>
       <c r="AI20" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ20" t="s">
         <v>95</v>
       </c>
-      <c r="AJ20" t="s">
-        <v>96</v>
-      </c>
       <c r="AK20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AL20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AM20" t="s">
         <v>16</v>
@@ -2922,13 +2956,13 @@
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21">
         <v>300</v>
@@ -2955,10 +2989,10 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -2985,7 +3019,7 @@
         <v>15</v>
       </c>
       <c r="V21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W21" t="s">
         <v>15</v>
@@ -2999,10 +3033,10 @@
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="C22" t="s">
         <v>39</v>
@@ -3032,10 +3066,10 @@
         <v>0</v>
       </c>
       <c r="L22" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="M22" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="N22">
         <v>-2</v>
@@ -3053,31 +3087,31 @@
         <v>28</v>
       </c>
       <c r="S22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W22" t="s">
         <v>15</v>
       </c>
       <c r="X22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Y22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Z22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AA22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB22" t="s">
         <v>16</v>
@@ -3085,10 +3119,10 @@
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="C23" t="s">
         <v>39</v>
@@ -3118,10 +3152,10 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="M23" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="N23">
         <v>-2</v>
@@ -3139,31 +3173,31 @@
         <v>28</v>
       </c>
       <c r="S23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T23" t="s">
         <v>15</v>
       </c>
       <c r="U23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W23" t="s">
         <v>15</v>
       </c>
       <c r="X23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Y23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Z23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AA23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB23" t="s">
         <v>16</v>
@@ -3171,55 +3205,55 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D24">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
         <v>0.8</v>
       </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="M24" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="N24">
-        <v>-2</v>
+        <v>0.5</v>
       </c>
       <c r="O24">
         <v>2</v>
       </c>
       <c r="P24">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Q24">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="R24" t="s">
         <v>28</v>
@@ -3228,75 +3262,69 @@
         <v>14</v>
       </c>
       <c r="T24" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="U24" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="V24" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="W24" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="X24" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="Y24" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="Z24" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="AA24" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="AB24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC24" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="AD24" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="AE24" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG24" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D25">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G25">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I25">
-        <v>0.8</v>
+        <v>1.5</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -3305,81 +3333,66 @@
         <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="M25" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="N25">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="O25">
         <v>0.5</v>
       </c>
       <c r="P25">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="Q25">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="R25" t="s">
         <v>28</v>
       </c>
       <c r="S25" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="T25" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="U25" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="V25" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="W25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="X25" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="Y25" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="Z25" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AA25" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="AB25" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF25" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26">
         <v>170</v>
@@ -3388,7 +3401,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>1.25</v>
@@ -3406,7 +3419,7 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="M26" t="s">
         <v>33</v>
@@ -3415,13 +3428,13 @@
         <v>-2</v>
       </c>
       <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26">
         <v>-1</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <v>0.5</v>
-      </c>
-      <c r="Q26">
-        <v>2</v>
       </c>
       <c r="R26" t="s">
         <v>28</v>
@@ -3430,16 +3443,16 @@
         <v>14</v>
       </c>
       <c r="T26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U26" t="s">
         <v>15</v>
       </c>
       <c r="V26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="X26" t="s">
         <v>15</v>
@@ -3448,10 +3461,10 @@
         <v>49</v>
       </c>
       <c r="Z26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AB26" t="s">
         <v>15</v>
@@ -3474,13 +3487,13 @@
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
         <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27">
         <v>170</v>
@@ -3489,25 +3502,25 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="J27">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="M27" t="s">
         <v>33</v>
@@ -3516,13 +3529,13 @@
         <v>-2</v>
       </c>
       <c r="O27">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q27">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R27" t="s">
         <v>28</v>
@@ -3531,27 +3544,60 @@
         <v>14</v>
       </c>
       <c r="T27" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="U27" t="s">
         <v>15</v>
       </c>
       <c r="V27" t="s">
+        <v>57</v>
+      </c>
+      <c r="W27" t="s">
+        <v>64</v>
+      </c>
+      <c r="X27" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -3560,13 +3606,13 @@
         <v>2</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -3575,45 +3621,215 @@
         <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="M28" t="s">
         <v>33</v>
       </c>
       <c r="N28">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="O28">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P28">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R28" t="s">
         <v>28</v>
       </c>
       <c r="S28" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="T28" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="U28" t="s">
         <v>15</v>
       </c>
       <c r="V28" t="s">
+        <v>57</v>
+      </c>
+      <c r="W28" t="s">
+        <v>61</v>
+      </c>
+      <c r="X28" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG28" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29">
+        <v>170</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>1.5</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0.4</v>
+      </c>
+      <c r="J29">
+        <v>0.9</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29" t="s">
+        <v>120</v>
+      </c>
+      <c r="M29" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29">
+        <v>-2</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29" t="s">
+        <v>28</v>
+      </c>
+      <c r="S29" t="s">
+        <v>14</v>
+      </c>
+      <c r="T29" t="s">
+        <v>15</v>
+      </c>
+      <c r="U29" t="s">
+        <v>15</v>
+      </c>
+      <c r="V29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30">
+        <v>75</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30" t="s">
+        <v>120</v>
+      </c>
+      <c r="M30" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30">
+        <v>2</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30" t="s">
+        <v>28</v>
+      </c>
+      <c r="S30" t="s">
+        <v>59</v>
+      </c>
+      <c r="T30" t="s">
+        <v>15</v>
+      </c>
+      <c r="U30" t="s">
+        <v>15</v>
+      </c>
+      <c r="V30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added placeholder texts for almost all battle interrupts, almost final balancing
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3A5FE1-30D9-4E83-B072-04F263CB4FF1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E1C148-6A09-47E5-85A2-984B45069A76}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="130">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -88,9 +88,6 @@
     <t>frog_mario</t>
   </si>
   <si>
-    <t>bolt wk/res</t>
-  </si>
-  <si>
     <t>aimed</t>
   </si>
   <si>
@@ -395,6 +392,24 @@
   </si>
   <si>
     <t>widened</t>
+  </si>
+  <si>
+    <t>Obviously A Cat</t>
+  </si>
+  <si>
+    <t>spr_bt_cat</t>
+  </si>
+  <si>
+    <t>Catsune</t>
+  </si>
+  <si>
+    <t>HealthLow1,Catsune,false</t>
+  </si>
+  <si>
+    <t>splash</t>
+  </si>
+  <si>
+    <t>volt wk/res</t>
   </si>
 </sst>
 </file>
@@ -1242,13 +1257,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM31"/>
+  <dimension ref="A1:AP33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y25" sqref="Y25"/>
+      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,7 +1296,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1299,34 +1314,34 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>7</v>
@@ -1347,7 +1362,7 @@
         <v>12</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
@@ -1358,7 +1373,7 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -1385,10 +1400,10 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -1403,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S2" t="s">
         <v>14</v>
@@ -1415,7 +1430,7 @@
         <v>15</v>
       </c>
       <c r="V2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W2" t="s">
         <v>15</v>
@@ -1424,10 +1439,10 @@
         <v>15</v>
       </c>
       <c r="Y2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA2" t="s">
         <v>15</v>
@@ -1447,7 +1462,7 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -1474,10 +1489,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N3">
         <v>-1</v>
@@ -1492,7 +1507,7 @@
         <v>-2</v>
       </c>
       <c r="R3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S3" t="s">
         <v>14</v>
@@ -1504,19 +1519,19 @@
         <v>15</v>
       </c>
       <c r="V3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X3" t="s">
         <v>15</v>
       </c>
       <c r="Y3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA3" t="s">
         <v>15</v>
@@ -1530,13 +1545,13 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>100</v>
@@ -1563,10 +1578,10 @@
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N4">
         <v>1.2</v>
@@ -1581,31 +1596,31 @@
         <v>1</v>
       </c>
       <c r="R4" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y4" t="s">
         <v>28</v>
       </c>
-      <c r="S4" t="s">
-        <v>57</v>
-      </c>
-      <c r="T4" t="s">
-        <v>15</v>
-      </c>
-      <c r="U4" t="s">
-        <v>15</v>
-      </c>
-      <c r="V4" t="s">
-        <v>57</v>
-      </c>
-      <c r="W4" t="s">
-        <v>15</v>
-      </c>
-      <c r="X4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>29</v>
-      </c>
       <c r="Z4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA4" t="s">
         <v>15</v>
@@ -1619,13 +1634,13 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>35</v>
@@ -1652,31 +1667,31 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N5">
         <v>0.75</v>
       </c>
       <c r="O5">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="P5">
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="Q5">
         <v>1.5</v>
       </c>
       <c r="R5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U5" t="s">
         <v>15</v>
@@ -1685,31 +1700,31 @@
         <v>14</v>
       </c>
       <c r="W5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X5" t="s">
         <v>15</v>
       </c>
       <c r="Y5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB5" t="s">
         <v>15</v>
       </c>
       <c r="AC5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AD5" t="s">
         <v>14</v>
       </c>
       <c r="AE5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF5" t="s">
         <v>15</v>
@@ -1720,13 +1735,13 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <v>18</v>
@@ -1753,10 +1768,10 @@
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -1771,7 +1786,7 @@
         <v>2</v>
       </c>
       <c r="R6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S6" t="s">
         <v>14</v>
@@ -1788,13 +1803,13 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7">
         <v>90</v>
@@ -1821,10 +1836,10 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -1839,10 +1854,10 @@
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T7" t="s">
         <v>15</v>
@@ -1859,10 +1874,10 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>28</v>
@@ -1889,10 +1904,10 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1907,10 +1922,10 @@
         <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T8" t="s">
         <v>15</v>
@@ -1924,13 +1939,13 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>30</v>
@@ -1957,10 +1972,10 @@
         <v>15</v>
       </c>
       <c r="L9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1975,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S9" t="s">
         <v>14</v>
@@ -1987,7 +2002,7 @@
         <v>15</v>
       </c>
       <c r="V9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W9" t="s">
         <v>15</v>
@@ -2001,13 +2016,13 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
         <v>73</v>
       </c>
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -2034,10 +2049,10 @@
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2046,16 +2061,16 @@
         <v>-1</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q10">
         <v>2</v>
       </c>
       <c r="R10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T10" t="s">
         <v>15</v>
@@ -2067,7 +2082,7 @@
         <v>14</v>
       </c>
       <c r="W10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X10" t="s">
         <v>15</v>
@@ -2078,13 +2093,13 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11">
         <v>100</v>
@@ -2111,10 +2126,10 @@
         <v>10</v>
       </c>
       <c r="L11" t="s">
+        <v>97</v>
+      </c>
+      <c r="M11" t="s">
         <v>98</v>
-      </c>
-      <c r="M11" t="s">
-        <v>99</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -2129,7 +2144,7 @@
         <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S11" t="s">
         <v>14</v>
@@ -2146,13 +2161,13 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12">
         <v>150</v>
@@ -2179,10 +2194,10 @@
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -2197,10 +2212,10 @@
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T12" t="s">
         <v>15</v>
@@ -2214,16 +2229,16 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2247,10 +2262,10 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -2265,22 +2280,22 @@
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S13" t="s">
         <v>14</v>
       </c>
       <c r="T13" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="U13" t="s">
         <v>15</v>
       </c>
       <c r="V13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W13" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="X13" t="s">
         <v>15</v>
@@ -2291,31 +2306,31 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14">
-        <v>1.3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -2324,16 +2339,16 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P14">
         <v>-1</v>
@@ -2342,22 +2357,22 @@
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S14" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="T14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U14" t="s">
         <v>15</v>
       </c>
       <c r="V14" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="W14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X14" t="s">
         <v>15</v>
@@ -2368,13 +2383,13 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15">
         <v>45</v>
@@ -2401,10 +2416,10 @@
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -2419,13 +2434,13 @@
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U15" t="s">
         <v>15</v>
@@ -2434,7 +2449,7 @@
         <v>14</v>
       </c>
       <c r="W15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X15" t="s">
         <v>15</v>
@@ -2445,13 +2460,13 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
         <v>83</v>
       </c>
-      <c r="B16" t="s">
-        <v>84</v>
-      </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16">
         <v>65</v>
@@ -2478,10 +2493,10 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N16">
         <v>0.75</v>
@@ -2496,22 +2511,22 @@
         <v>-1</v>
       </c>
       <c r="R16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U16" t="s">
         <v>15</v>
       </c>
       <c r="V16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X16" t="s">
         <v>15</v>
@@ -2520,15 +2535,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17">
         <v>300</v>
@@ -2555,10 +2570,10 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -2573,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="R17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S17" t="s">
         <v>14</v>
@@ -2585,7 +2600,7 @@
         <v>15</v>
       </c>
       <c r="V17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W17" t="s">
         <v>15</v>
@@ -2594,10 +2609,10 @@
         <v>15</v>
       </c>
       <c r="Y17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA17" t="s">
         <v>15</v>
@@ -2609,63 +2624,63 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="D18">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>0.7</v>
       </c>
       <c r="J18">
-        <v>1.5</v>
+        <v>0.9</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L18" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="M18" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S18" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="T18" t="s">
         <v>15</v>
@@ -2674,66 +2689,27 @@
         <v>15</v>
       </c>
       <c r="V18" t="s">
-        <v>109</v>
-      </c>
-      <c r="W18" t="s">
-        <v>61</v>
-      </c>
-      <c r="X18" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19">
         <v>0.75</v>
@@ -2751,16 +2727,16 @@
         <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N19">
         <v>-2</v>
       </c>
       <c r="O19">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="P19">
         <v>-2</v>
@@ -2769,203 +2745,200 @@
         <v>2</v>
       </c>
       <c r="R19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S19" t="s">
         <v>14</v>
       </c>
       <c r="T19" t="s">
+        <v>15</v>
+      </c>
+      <c r="U19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" t="s">
+        <v>56</v>
+      </c>
+      <c r="W19" t="s">
+        <v>62</v>
+      </c>
+      <c r="X19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO19" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>300</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <v>1.5</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" t="s">
+        <v>32</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="R20" t="s">
+        <v>27</v>
+      </c>
+      <c r="S20" t="s">
+        <v>105</v>
+      </c>
+      <c r="T20" t="s">
+        <v>15</v>
+      </c>
+      <c r="U20" t="s">
+        <v>15</v>
+      </c>
+      <c r="V20" t="s">
+        <v>108</v>
+      </c>
+      <c r="W20" t="s">
+        <v>60</v>
+      </c>
+      <c r="X20" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
         <v>64</v>
       </c>
-      <c r="U19" t="s">
-        <v>15</v>
-      </c>
-      <c r="V19" t="s">
-        <v>57</v>
-      </c>
-      <c r="W19" t="s">
-        <v>63</v>
-      </c>
-      <c r="X19" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ19" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK19" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20">
-        <v>150</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>0.75</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0.7</v>
-      </c>
-      <c r="J20">
-        <v>0.9</v>
-      </c>
-      <c r="K20">
-        <v>10</v>
-      </c>
-      <c r="L20" t="s">
-        <v>92</v>
-      </c>
-      <c r="M20" t="s">
-        <v>33</v>
-      </c>
-      <c r="N20">
-        <v>-2</v>
-      </c>
-      <c r="O20">
-        <v>2</v>
-      </c>
-      <c r="P20">
-        <v>-2</v>
-      </c>
-      <c r="Q20">
-        <v>-2</v>
-      </c>
-      <c r="R20" t="s">
-        <v>28</v>
-      </c>
-      <c r="S20" t="s">
-        <v>14</v>
-      </c>
-      <c r="T20" t="s">
-        <v>61</v>
-      </c>
-      <c r="U20" t="s">
-        <v>15</v>
-      </c>
-      <c r="V20" t="s">
-        <v>14</v>
-      </c>
-      <c r="W20" t="s">
-        <v>15</v>
-      </c>
-      <c r="X20" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF20" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ20" t="s">
-        <v>95</v>
-      </c>
-      <c r="AK20" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL20" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
       <c r="D21">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -2977,69 +2950,111 @@
         <v>0.75</v>
       </c>
       <c r="H21">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L21" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="M21" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="O21">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="P21">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="Q21">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="R21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S21" t="s">
         <v>14</v>
       </c>
       <c r="T21" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="U21" t="s">
         <v>15</v>
       </c>
       <c r="V21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W21" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="X21" t="s">
         <v>15</v>
       </c>
       <c r="Y21" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="D22">
         <v>150</v>
@@ -3051,31 +3066,31 @@
         <v>2</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L22" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="M22" t="s">
-        <v>122</v>
+        <v>32</v>
       </c>
       <c r="N22">
         <v>-2</v>
       </c>
       <c r="O22">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="P22">
         <v>-2</v>
@@ -3084,229 +3099,244 @@
         <v>-2</v>
       </c>
       <c r="R22" t="s">
+        <v>27</v>
+      </c>
+      <c r="S22" t="s">
+        <v>14</v>
+      </c>
+      <c r="T22" t="s">
+        <v>60</v>
+      </c>
+      <c r="U22" t="s">
+        <v>15</v>
+      </c>
+      <c r="V22" t="s">
+        <v>14</v>
+      </c>
+      <c r="W22" t="s">
+        <v>15</v>
+      </c>
+      <c r="X22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB22" t="s">
         <v>28</v>
       </c>
-      <c r="S22" t="s">
-        <v>76</v>
-      </c>
-      <c r="T22" t="s">
-        <v>63</v>
-      </c>
-      <c r="U22" t="s">
-        <v>115</v>
-      </c>
-      <c r="V22" t="s">
-        <v>76</v>
-      </c>
-      <c r="W22" t="s">
-        <v>15</v>
-      </c>
-      <c r="X22" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB22" t="s">
+      <c r="AC22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23">
+        <v>300</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>0.75</v>
+      </c>
+      <c r="H23">
+        <v>0.1</v>
+      </c>
+      <c r="I23">
+        <v>0.5</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>97</v>
+      </c>
+      <c r="M23" t="s">
+        <v>111</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0.5</v>
+      </c>
+      <c r="P23">
+        <v>0.5</v>
+      </c>
+      <c r="Q23">
+        <v>0.5</v>
+      </c>
+      <c r="R23" t="s">
+        <v>27</v>
+      </c>
+      <c r="S23" t="s">
+        <v>14</v>
+      </c>
+      <c r="T23" t="s">
+        <v>15</v>
+      </c>
+      <c r="U23" t="s">
+        <v>15</v>
+      </c>
+      <c r="V23" t="s">
+        <v>56</v>
+      </c>
+      <c r="W23" t="s">
+        <v>15</v>
+      </c>
+      <c r="X23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24">
+        <v>150</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0.5</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>120</v>
+      </c>
+      <c r="M24" t="s">
+        <v>121</v>
+      </c>
+      <c r="N24">
+        <v>-2</v>
+      </c>
+      <c r="O24">
+        <v>-2</v>
+      </c>
+      <c r="P24">
+        <v>-2</v>
+      </c>
+      <c r="Q24">
+        <v>-2</v>
+      </c>
+      <c r="R24" t="s">
+        <v>27</v>
+      </c>
+      <c r="S24" t="s">
+        <v>75</v>
+      </c>
+      <c r="T24" t="s">
+        <v>62</v>
+      </c>
+      <c r="U24" t="s">
         <v>114</v>
       </c>
-      <c r="B23" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23">
-        <v>150</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0.9</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>121</v>
-      </c>
-      <c r="M23" t="s">
-        <v>123</v>
-      </c>
-      <c r="N23">
-        <v>-2</v>
-      </c>
-      <c r="O23">
-        <v>-2</v>
-      </c>
-      <c r="P23">
-        <v>-2</v>
-      </c>
-      <c r="Q23">
-        <v>-2</v>
-      </c>
-      <c r="R23" t="s">
-        <v>28</v>
-      </c>
-      <c r="S23" t="s">
-        <v>76</v>
-      </c>
-      <c r="T23" t="s">
-        <v>15</v>
-      </c>
-      <c r="U23" t="s">
-        <v>115</v>
-      </c>
-      <c r="V23" t="s">
-        <v>76</v>
-      </c>
-      <c r="W23" t="s">
-        <v>15</v>
-      </c>
-      <c r="X23" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB23" t="s">
+      <c r="V24" t="s">
+        <v>75</v>
+      </c>
+      <c r="W24" t="s">
+        <v>15</v>
+      </c>
+      <c r="X24" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" t="s">
-        <v>116</v>
-      </c>
-      <c r="C24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24">
-        <v>100</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24">
-        <v>1.5</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="J24">
-        <v>0.8</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
-        <v>92</v>
-      </c>
-      <c r="M24" t="s">
-        <v>116</v>
-      </c>
-      <c r="N24">
-        <v>0.5</v>
-      </c>
-      <c r="O24">
-        <v>2</v>
-      </c>
-      <c r="P24">
-        <v>2</v>
-      </c>
-      <c r="Q24">
-        <v>2</v>
-      </c>
-      <c r="R24" t="s">
-        <v>28</v>
-      </c>
-      <c r="S24" t="s">
-        <v>14</v>
-      </c>
-      <c r="T24" t="s">
-        <v>15</v>
-      </c>
-      <c r="U24" t="s">
-        <v>96</v>
-      </c>
-      <c r="V24" t="s">
-        <v>14</v>
-      </c>
-      <c r="W24" t="s">
-        <v>15</v>
-      </c>
-      <c r="X24" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25">
         <v>150</v>
@@ -3315,16 +3345,16 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G25">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>1.5</v>
+        <v>0.9</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -3333,185 +3363,179 @@
         <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="M25" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="N25">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="O25">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="P25">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="Q25">
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="R25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S25" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="T25" t="s">
         <v>15</v>
       </c>
       <c r="U25" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="V25" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="W25" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="X25" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="Y25" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="Z25" t="s">
         <v>63</v>
       </c>
       <c r="AA25" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="AB25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D26">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
         <v>0.8</v>
       </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="M26" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="N26">
-        <v>-2</v>
+        <v>0.5</v>
       </c>
       <c r="O26">
         <v>2</v>
       </c>
       <c r="P26">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Q26">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="R26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S26" t="s">
         <v>14</v>
       </c>
       <c r="T26" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="U26" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="V26" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="W26" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="X26" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="Y26" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="Z26" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="AA26" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="AB26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC26" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="AD26" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="AE26" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF26" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D27">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G27">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I27">
-        <v>0.8</v>
+        <v>1.5</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -3520,81 +3544,66 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="M27" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="N27">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="O27">
         <v>0.5</v>
       </c>
       <c r="P27">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="Q27">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="R27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S27" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="T27" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="U27" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="V27" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="W27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="X27" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="Y27" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="Z27" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="AA27" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="AB27" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>51</v>
       </c>
-      <c r="AE27" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>54</v>
-      </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28">
         <v>170</v>
@@ -3603,7 +3612,7 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <v>1.25</v>
@@ -3621,61 +3630,61 @@
         <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N28">
         <v>-2</v>
       </c>
       <c r="O28">
+        <v>2</v>
+      </c>
+      <c r="P28">
         <v>-1</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>0.5</v>
       </c>
-      <c r="Q28">
-        <v>2</v>
-      </c>
       <c r="R28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S28" t="s">
         <v>14</v>
       </c>
       <c r="T28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U28" t="s">
         <v>15</v>
       </c>
       <c r="V28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X28" t="s">
         <v>15</v>
       </c>
       <c r="Y28" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC28" t="s">
         <v>49</v>
       </c>
-      <c r="Z28" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC28" t="s">
+      <c r="AD28" t="s">
         <v>50</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>51</v>
       </c>
       <c r="AE28" t="s">
         <v>15</v>
@@ -3687,15 +3696,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
         <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29">
         <v>170</v>
@@ -3704,127 +3713,329 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="J29">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N29">
         <v>-2</v>
       </c>
       <c r="O29">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q29">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S29" t="s">
         <v>14</v>
       </c>
       <c r="T29" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="U29" t="s">
         <v>15</v>
       </c>
       <c r="V29" t="s">
+        <v>56</v>
+      </c>
+      <c r="W29" t="s">
+        <v>63</v>
+      </c>
+      <c r="X29" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30">
+        <v>170</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>1.25</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0.8</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30" t="s">
+        <v>119</v>
+      </c>
+      <c r="M30" t="s">
+        <v>32</v>
+      </c>
+      <c r="N30">
+        <v>-2</v>
+      </c>
+      <c r="O30">
+        <v>-1</v>
+      </c>
+      <c r="P30">
+        <v>0.5</v>
+      </c>
+      <c r="Q30">
+        <v>2</v>
+      </c>
+      <c r="R30" t="s">
+        <v>27</v>
+      </c>
+      <c r="S30" t="s">
+        <v>14</v>
+      </c>
+      <c r="T30" t="s">
+        <v>60</v>
+      </c>
+      <c r="U30" t="s">
+        <v>15</v>
+      </c>
+      <c r="V30" t="s">
+        <v>56</v>
+      </c>
+      <c r="W30" t="s">
+        <v>60</v>
+      </c>
+      <c r="X30" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>67</v>
       </c>
-      <c r="D30">
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31">
+        <v>170</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>1.5</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0.4</v>
+      </c>
+      <c r="J31">
+        <v>0.9</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31" t="s">
+        <v>119</v>
+      </c>
+      <c r="M31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N31">
+        <v>-2</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31" t="s">
+        <v>27</v>
+      </c>
+      <c r="S31" t="s">
+        <v>14</v>
+      </c>
+      <c r="T31" t="s">
+        <v>15</v>
+      </c>
+      <c r="U31" t="s">
+        <v>15</v>
+      </c>
+      <c r="V31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32">
         <v>75</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>2</v>
-      </c>
-      <c r="G30">
-        <v>2</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
         <v>3</v>
       </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30" t="s">
-        <v>120</v>
-      </c>
-      <c r="M30" t="s">
-        <v>33</v>
-      </c>
-      <c r="N30">
-        <v>2</v>
-      </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30" t="s">
-        <v>28</v>
-      </c>
-      <c r="S30" t="s">
-        <v>59</v>
-      </c>
-      <c r="T30" t="s">
-        <v>15</v>
-      </c>
-      <c r="U30" t="s">
-        <v>15</v>
-      </c>
-      <c r="V30" t="s">
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32" t="s">
+        <v>119</v>
+      </c>
+      <c r="M32" t="s">
+        <v>32</v>
+      </c>
+      <c r="N32">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32" t="s">
+        <v>27</v>
+      </c>
+      <c r="S32" t="s">
+        <v>58</v>
+      </c>
+      <c r="T32" t="s">
+        <v>15</v>
+      </c>
+      <c r="U32" t="s">
+        <v>15</v>
+      </c>
+      <c r="V32" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nerfed tanuki to make the Ijiraq2 battle easier
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CE8A3F-6221-4169-870E-44E9B00D3DA0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EB2650-76C7-4775-858D-25D6D8DC8079}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="133">
   <si>
     <t>Name(ID)</t>
   </si>
@@ -232,9 +232,6 @@
     <t>selfcare</t>
   </si>
   <si>
-    <t>spr_bt_changeling_healer</t>
-  </si>
-  <si>
     <t>Wechselbalg</t>
   </si>
   <si>
@@ -373,12 +370,6 @@
     <t>spr_bt_doppelganger_dahlia</t>
   </si>
   <si>
-    <t>spr_bt_illyia</t>
-  </si>
-  <si>
-    <t>spr_bt_dahlia</t>
-  </si>
-  <si>
     <t>Doppelganger1</t>
   </si>
   <si>
@@ -416,6 +407,18 @@
   </si>
   <si>
     <t>powered</t>
+  </si>
+  <si>
+    <t>spr_bt_doppelganger</t>
+  </si>
+  <si>
+    <t>spr_bt_wechselbalg</t>
+  </si>
+  <si>
+    <t>spr_bt_illusion_illyia</t>
+  </si>
+  <si>
+    <t>spr_bt_illusion_dahlia</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1272,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1344,7 +1347,7 @@
         <v>61</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>24</v>
@@ -1498,7 +1501,7 @@
         <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N3">
         <v>-1</v>
@@ -1724,7 +1727,7 @@
         <v>15</v>
       </c>
       <c r="AC5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AD5" t="s">
         <v>14</v>
@@ -1809,13 +1812,13 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7">
         <v>90</v>
@@ -1895,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -2022,13 +2025,13 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
         <v>72</v>
       </c>
-      <c r="B10" t="s">
-        <v>73</v>
-      </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -2076,7 +2079,7 @@
         <v>27</v>
       </c>
       <c r="S10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T10" t="s">
         <v>15</v>
@@ -2099,7 +2102,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
@@ -2132,10 +2135,10 @@
         <v>10</v>
       </c>
       <c r="L11" t="s">
+        <v>96</v>
+      </c>
+      <c r="M11" t="s">
         <v>97</v>
-      </c>
-      <c r="M11" t="s">
-        <v>98</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -2167,7 +2170,7 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
         <v>42</v>
@@ -2200,10 +2203,10 @@
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -2238,7 +2241,7 @@
         <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
         <v>65</v>
@@ -2315,7 +2318,7 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
         <v>65</v>
@@ -2392,7 +2395,7 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
         <v>65</v>
@@ -2466,10 +2469,10 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
         <v>82</v>
-      </c>
-      <c r="B16" t="s">
-        <v>83</v>
       </c>
       <c r="C16" t="s">
         <v>64</v>
@@ -2529,7 +2532,7 @@
         <v>15</v>
       </c>
       <c r="V16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W16" t="s">
         <v>63</v>
@@ -2543,10 +2546,10 @@
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -2576,10 +2579,10 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -2632,10 +2635,10 @@
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C18" t="s">
         <v>64</v>
@@ -2665,10 +2668,10 @@
         <v>10</v>
       </c>
       <c r="L18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -2686,7 +2689,7 @@
         <v>27</v>
       </c>
       <c r="S18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="T18" t="s">
         <v>15</v>
@@ -2700,10 +2703,10 @@
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
         <v>64</v>
@@ -2733,7 +2736,7 @@
         <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M19" t="s">
         <v>32</v>
@@ -2772,7 +2775,7 @@
         <v>15</v>
       </c>
       <c r="Y19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Z19" t="s">
         <v>15</v>
@@ -2793,7 +2796,7 @@
         <v>28</v>
       </c>
       <c r="AF19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AG19" t="s">
         <v>15</v>
@@ -2811,7 +2814,7 @@
         <v>15</v>
       </c>
       <c r="AL19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM19" t="s">
         <v>69</v>
@@ -2828,10 +2831,10 @@
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
@@ -2882,7 +2885,7 @@
         <v>27</v>
       </c>
       <c r="S20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T20" t="s">
         <v>15</v>
@@ -2891,25 +2894,25 @@
         <v>15</v>
       </c>
       <c r="V20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W20" t="s">
         <v>60</v>
       </c>
       <c r="X20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z20" t="s">
         <v>15</v>
       </c>
       <c r="AA20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AB20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AC20" t="s">
         <v>15</v>
@@ -2921,7 +2924,7 @@
         <v>28</v>
       </c>
       <c r="AF20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AG20" t="s">
         <v>15</v>
@@ -2935,10 +2938,10 @@
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
         <v>64</v>
@@ -2968,7 +2971,7 @@
         <v>10</v>
       </c>
       <c r="L21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M21" t="s">
         <v>32</v>
@@ -3007,7 +3010,7 @@
         <v>15</v>
       </c>
       <c r="Y21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Z21" t="s">
         <v>15</v>
@@ -3019,7 +3022,7 @@
         <v>28</v>
       </c>
       <c r="AC21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AD21" t="s">
         <v>15</v>
@@ -3037,7 +3040,7 @@
         <v>15</v>
       </c>
       <c r="AI21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AJ21" t="s">
         <v>69</v>
@@ -3046,7 +3049,7 @@
         <v>60</v>
       </c>
       <c r="AL21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AM21" t="s">
         <v>16</v>
@@ -3054,10 +3057,10 @@
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
         <v>64</v>
@@ -3087,7 +3090,7 @@
         <v>10</v>
       </c>
       <c r="L22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M22" t="s">
         <v>32</v>
@@ -3156,16 +3159,16 @@
         <v>15</v>
       </c>
       <c r="AI22" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ22" t="s">
         <v>93</v>
-      </c>
-      <c r="AJ22" t="s">
-        <v>94</v>
       </c>
       <c r="AK22" t="s">
         <v>62</v>
       </c>
       <c r="AL22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AM22" t="s">
         <v>16</v>
@@ -3173,10 +3176,10 @@
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="C23" t="s">
         <v>66</v>
@@ -3206,10 +3209,10 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -3250,10 +3253,10 @@
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -3283,10 +3286,10 @@
         <v>0</v>
       </c>
       <c r="L24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="M24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="N24">
         <v>-2</v>
@@ -3304,31 +3307,31 @@
         <v>27</v>
       </c>
       <c r="S24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T24" t="s">
         <v>62</v>
       </c>
       <c r="U24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W24" t="s">
         <v>15</v>
       </c>
       <c r="X24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Z24" t="s">
         <v>62</v>
       </c>
       <c r="AA24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AB24" t="s">
         <v>16</v>
@@ -3336,10 +3339,10 @@
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
@@ -3369,10 +3372,10 @@
         <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="M25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N25">
         <v>-2</v>
@@ -3390,31 +3393,31 @@
         <v>27</v>
       </c>
       <c r="S25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T25" t="s">
         <v>15</v>
       </c>
       <c r="U25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W25" t="s">
         <v>63</v>
       </c>
       <c r="X25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Z25" t="s">
         <v>63</v>
       </c>
       <c r="AA25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AB25" t="s">
         <v>16</v>
@@ -3422,10 +3425,10 @@
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
@@ -3455,10 +3458,10 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N26">
         <v>0.5</v>
@@ -3482,7 +3485,7 @@
         <v>15</v>
       </c>
       <c r="U26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="V26" t="s">
         <v>14</v>
@@ -3491,16 +3494,16 @@
         <v>15</v>
       </c>
       <c r="X26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Z26" t="s">
         <v>15</v>
       </c>
       <c r="AA26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AB26" t="s">
         <v>14</v>
@@ -3509,7 +3512,7 @@
         <v>15</v>
       </c>
       <c r="AD26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AE26" t="s">
         <v>16</v>
@@ -3517,10 +3520,10 @@
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
         <v>38</v>
@@ -3550,10 +3553,10 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -3577,7 +3580,7 @@
         <v>60</v>
       </c>
       <c r="U27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="V27" t="s">
         <v>69</v>
@@ -3586,7 +3589,7 @@
         <v>15</v>
       </c>
       <c r="X27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Y27" t="s">
         <v>58</v>
@@ -3595,7 +3598,7 @@
         <v>15</v>
       </c>
       <c r="AA27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AB27" t="s">
         <v>16</v>
@@ -3606,7 +3609,7 @@
         <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
         <v>66</v>
@@ -3636,7 +3639,7 @@
         <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M28" t="s">
         <v>32</v>
@@ -3707,7 +3710,7 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
         <v>66</v>
@@ -3737,7 +3740,7 @@
         <v>0</v>
       </c>
       <c r="L29" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M29" t="s">
         <v>32</v>
@@ -3808,7 +3811,7 @@
         <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
         <v>66</v>
@@ -3838,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="L30" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M30" t="s">
         <v>32</v>
@@ -3909,7 +3912,7 @@
         <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
         <v>66</v>
@@ -3939,7 +3942,7 @@
         <v>0</v>
       </c>
       <c r="L31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M31" t="s">
         <v>32</v>
@@ -3977,7 +3980,7 @@
         <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
         <v>66</v>
@@ -4007,7 +4010,7 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M32" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Added and Tested incubator assets
-Added and tested new BGs, character sprites, codec sprites, and battle sprites.
-Changed location of left codec to account for un-cropped JT sprites
-I left the test changes in the gameflow prefab in case others wanted to look at them, but did not update the prefab. Feel free to revert
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/enemyDatabase.xlsx
+++ b/Typocrypha/Assets/excel/enemyDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\GitHub\typocrypha\Typocrypha\Assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EB2650-76C7-4775-858D-25D6D8DC8079}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87721E54-8DFE-4B7F-BFD9-2C5D1DE97865}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enemyDatabase" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>Changeling</t>
   </si>
   <si>
-    <t>spr_bt_tanuki</t>
-  </si>
-  <si>
     <t>spr_bt_ladon</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t>Doppelganger (???)</t>
   </si>
   <si>
-    <t>spr_bt_changeling</t>
-  </si>
-  <si>
     <t>selfcare</t>
   </si>
   <si>
@@ -238,12 +232,6 @@
     <t>Bunbuku</t>
   </si>
   <si>
-    <t>spr_bt_tanuki_fire</t>
-  </si>
-  <si>
-    <t>spr_bt_ijiraq</t>
-  </si>
-  <si>
     <t>stress</t>
   </si>
   <si>
@@ -419,6 +407,18 @@
   </si>
   <si>
     <t>spr_bt_illusion_dahlia</t>
+  </si>
+  <si>
+    <t>spr_bt_ijiraq_new</t>
+  </si>
+  <si>
+    <t>spr_bt_tanooki_new</t>
+  </si>
+  <si>
+    <t>spr_bt_tanooki_fire</t>
+  </si>
+  <si>
+    <t>spr_bt_changeling_new</t>
   </si>
 </sst>
 </file>
@@ -1269,16 +1269,17 @@
   <dimension ref="A1:AP33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="3" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="12" max="12" width="12.33203125" customWidth="1"/>
@@ -1341,13 +1342,13 @@
         <v>6</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>24</v>
@@ -1439,7 +1440,7 @@
         <v>15</v>
       </c>
       <c r="V2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W2" t="s">
         <v>15</v>
@@ -1501,7 +1502,7 @@
         <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="N3">
         <v>-1</v>
@@ -1528,10 +1529,10 @@
         <v>15</v>
       </c>
       <c r="V3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X3" t="s">
         <v>15</v>
@@ -1557,7 +1558,7 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
@@ -1608,7 +1609,7 @@
         <v>27</v>
       </c>
       <c r="S4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T4" t="s">
         <v>15</v>
@@ -1617,7 +1618,7 @@
         <v>15</v>
       </c>
       <c r="V4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W4" t="s">
         <v>15</v>
@@ -1629,7 +1630,7 @@
         <v>28</v>
       </c>
       <c r="Z4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA4" t="s">
         <v>15</v>
@@ -1646,7 +1647,7 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -1700,7 +1701,7 @@
         <v>14</v>
       </c>
       <c r="T5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U5" t="s">
         <v>15</v>
@@ -1718,22 +1719,22 @@
         <v>28</v>
       </c>
       <c r="Z5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB5" t="s">
         <v>15</v>
       </c>
       <c r="AC5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AD5" t="s">
         <v>14</v>
       </c>
       <c r="AE5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AF5" t="s">
         <v>15</v>
@@ -1747,10 +1748,10 @@
         <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>18</v>
@@ -1812,13 +1813,13 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D7">
         <v>90</v>
@@ -1866,7 +1867,7 @@
         <v>27</v>
       </c>
       <c r="S7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T7" t="s">
         <v>15</v>
@@ -1883,7 +1884,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
@@ -1934,7 +1935,7 @@
         <v>27</v>
       </c>
       <c r="S8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T8" t="s">
         <v>15</v>
@@ -1948,10 +1949,10 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
         <v>39</v>
@@ -2011,7 +2012,7 @@
         <v>15</v>
       </c>
       <c r="V9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W9" t="s">
         <v>15</v>
@@ -2025,13 +2026,13 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -2079,7 +2080,7 @@
         <v>27</v>
       </c>
       <c r="S10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="T10" t="s">
         <v>15</v>
@@ -2091,7 +2092,7 @@
         <v>14</v>
       </c>
       <c r="W10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X10" t="s">
         <v>15</v>
@@ -2102,10 +2103,10 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
         <v>39</v>
@@ -2135,10 +2136,10 @@
         <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -2170,10 +2171,10 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
@@ -2203,10 +2204,10 @@
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -2224,7 +2225,7 @@
         <v>27</v>
       </c>
       <c r="S12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T12" t="s">
         <v>15</v>
@@ -2238,13 +2239,13 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13">
         <v>40</v>
@@ -2301,7 +2302,7 @@
         <v>15</v>
       </c>
       <c r="V13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W13" t="s">
         <v>15</v>
@@ -2315,13 +2316,13 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -2372,16 +2373,16 @@
         <v>14</v>
       </c>
       <c r="T14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U14" t="s">
         <v>15</v>
       </c>
       <c r="V14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X14" t="s">
         <v>15</v>
@@ -2392,13 +2393,13 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15">
         <v>45</v>
@@ -2446,10 +2447,10 @@
         <v>27</v>
       </c>
       <c r="S15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U15" t="s">
         <v>15</v>
@@ -2458,7 +2459,7 @@
         <v>14</v>
       </c>
       <c r="W15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X15" t="s">
         <v>15</v>
@@ -2469,13 +2470,13 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16">
         <v>65</v>
@@ -2523,19 +2524,19 @@
         <v>27</v>
       </c>
       <c r="S16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U16" t="s">
         <v>15</v>
       </c>
       <c r="V16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="W16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X16" t="s">
         <v>15</v>
@@ -2546,10 +2547,10 @@
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -2579,10 +2580,10 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -2609,7 +2610,7 @@
         <v>15</v>
       </c>
       <c r="V17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W17" t="s">
         <v>15</v>
@@ -2635,13 +2636,13 @@
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18">
         <v>150</v>
@@ -2668,10 +2669,10 @@
         <v>10</v>
       </c>
       <c r="L18" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -2689,7 +2690,7 @@
         <v>27</v>
       </c>
       <c r="S18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="T18" t="s">
         <v>15</v>
@@ -2703,13 +2704,13 @@
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19">
         <v>150</v>
@@ -2736,7 +2737,7 @@
         <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M19" t="s">
         <v>32</v>
@@ -2766,16 +2767,16 @@
         <v>15</v>
       </c>
       <c r="V19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X19" t="s">
         <v>15</v>
       </c>
       <c r="Y19" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Z19" t="s">
         <v>15</v>
@@ -2784,10 +2785,10 @@
         <v>15</v>
       </c>
       <c r="AB19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AD19" t="s">
         <v>15</v>
@@ -2796,7 +2797,7 @@
         <v>28</v>
       </c>
       <c r="AF19" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AG19" t="s">
         <v>15</v>
@@ -2814,13 +2815,13 @@
         <v>15</v>
       </c>
       <c r="AL19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AM19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AN19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AO19" t="s">
         <v>15</v>
@@ -2831,10 +2832,10 @@
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
@@ -2885,34 +2886,34 @@
         <v>27</v>
       </c>
       <c r="S20" t="s">
+        <v>100</v>
+      </c>
+      <c r="T20" t="s">
+        <v>15</v>
+      </c>
+      <c r="U20" t="s">
+        <v>15</v>
+      </c>
+      <c r="V20" t="s">
+        <v>103</v>
+      </c>
+      <c r="W20" t="s">
+        <v>59</v>
+      </c>
+      <c r="X20" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y20" t="s">
         <v>104</v>
       </c>
-      <c r="T20" t="s">
-        <v>15</v>
-      </c>
-      <c r="U20" t="s">
-        <v>15</v>
-      </c>
-      <c r="V20" t="s">
-        <v>107</v>
-      </c>
-      <c r="W20" t="s">
-        <v>60</v>
-      </c>
-      <c r="X20" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>108</v>
-      </c>
       <c r="Z20" t="s">
         <v>15</v>
       </c>
       <c r="AA20" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="AB20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="AC20" t="s">
         <v>15</v>
@@ -2924,7 +2925,7 @@
         <v>28</v>
       </c>
       <c r="AF20" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="AG20" t="s">
         <v>15</v>
@@ -2938,13 +2939,13 @@
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="B21" t="s">
-        <v>87</v>
-      </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21">
         <v>100</v>
@@ -2971,7 +2972,7 @@
         <v>10</v>
       </c>
       <c r="L21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M21" t="s">
         <v>32</v>
@@ -2995,22 +2996,22 @@
         <v>14</v>
       </c>
       <c r="T21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U21" t="s">
         <v>15</v>
       </c>
       <c r="V21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X21" t="s">
         <v>15</v>
       </c>
       <c r="Y21" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Z21" t="s">
         <v>15</v>
@@ -3022,7 +3023,7 @@
         <v>28</v>
       </c>
       <c r="AC21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AD21" t="s">
         <v>15</v>
@@ -3040,16 +3041,16 @@
         <v>15</v>
       </c>
       <c r="AI21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AJ21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AK21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AL21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AM21" t="s">
         <v>16</v>
@@ -3057,13 +3058,13 @@
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" t="s">
         <v>84</v>
       </c>
-      <c r="B22" t="s">
-        <v>88</v>
-      </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22">
         <v>150</v>
@@ -3090,7 +3091,7 @@
         <v>10</v>
       </c>
       <c r="L22" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M22" t="s">
         <v>32</v>
@@ -3114,7 +3115,7 @@
         <v>14</v>
       </c>
       <c r="T22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U22" t="s">
         <v>15</v>
@@ -3129,10 +3130,10 @@
         <v>15</v>
       </c>
       <c r="Y22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Z22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA22" t="s">
         <v>15</v>
@@ -3141,10 +3142,10 @@
         <v>28</v>
       </c>
       <c r="AC22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AD22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE22" t="s">
         <v>15</v>
@@ -3159,16 +3160,16 @@
         <v>15</v>
       </c>
       <c r="AI22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AJ22" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AK22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AL22" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="AM22" t="s">
         <v>16</v>
@@ -3176,13 +3177,13 @@
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23">
         <v>300</v>
@@ -3209,10 +3210,10 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M23" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -3239,7 +3240,7 @@
         <v>15</v>
       </c>
       <c r="V23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W23" t="s">
         <v>15</v>
@@ -3253,10 +3254,10 @@
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -3286,10 +3287,10 @@
         <v>0</v>
       </c>
       <c r="L24" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="M24" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="N24">
         <v>-2</v>
@@ -3307,31 +3308,31 @@
         <v>27</v>
       </c>
       <c r="S24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="T24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U24" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="V24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="W24" t="s">
         <v>15</v>
       </c>
       <c r="X24" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Y24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="Z24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AA24" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AB24" t="s">
         <v>16</v>
@@ -3339,10 +3340,10 @@
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
@@ -3372,10 +3373,10 @@
         <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="M25" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="N25">
         <v>-2</v>
@@ -3393,31 +3394,31 @@
         <v>27</v>
       </c>
       <c r="S25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="T25" t="s">
         <v>15</v>
       </c>
       <c r="U25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="V25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="W25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Y25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="Z25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA25" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AB25" t="s">
         <v>16</v>
@@ -3425,10 +3426,10 @@
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
@@ -3458,10 +3459,10 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M26" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="N26">
         <v>0.5</v>
@@ -3485,7 +3486,7 @@
         <v>15</v>
       </c>
       <c r="U26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="V26" t="s">
         <v>14</v>
@@ -3494,16 +3495,16 @@
         <v>15</v>
       </c>
       <c r="X26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="Y26" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Z26" t="s">
         <v>15</v>
       </c>
       <c r="AA26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="AB26" t="s">
         <v>14</v>
@@ -3512,7 +3513,7 @@
         <v>15</v>
       </c>
       <c r="AD26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="AE26" t="s">
         <v>16</v>
@@ -3520,10 +3521,10 @@
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
         <v>38</v>
@@ -3553,10 +3554,10 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -3574,31 +3575,31 @@
         <v>27</v>
       </c>
       <c r="S27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U27" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="V27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W27" t="s">
         <v>15</v>
       </c>
       <c r="X27" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="Y27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Z27" t="s">
         <v>15</v>
       </c>
       <c r="AA27" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AB27" t="s">
         <v>16</v>
@@ -3606,13 +3607,13 @@
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28">
         <v>170</v>
@@ -3639,7 +3640,7 @@
         <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="M28" t="s">
         <v>32</v>
@@ -3663,37 +3664,37 @@
         <v>14</v>
       </c>
       <c r="T28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U28" t="s">
         <v>15</v>
       </c>
       <c r="V28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X28" t="s">
         <v>15</v>
       </c>
       <c r="Y28" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC28" t="s">
         <v>48</v>
       </c>
-      <c r="Z28" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC28" t="s">
+      <c r="AD28" t="s">
         <v>49</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>50</v>
       </c>
       <c r="AE28" t="s">
         <v>15</v>
@@ -3707,13 +3708,13 @@
     </row>
     <row r="29" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29">
         <v>170</v>
@@ -3740,7 +3741,7 @@
         <v>0</v>
       </c>
       <c r="L29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="M29" t="s">
         <v>32</v>
@@ -3764,37 +3765,37 @@
         <v>14</v>
       </c>
       <c r="T29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U29" t="s">
         <v>15</v>
       </c>
       <c r="V29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X29" t="s">
         <v>15</v>
       </c>
       <c r="Y29" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC29" t="s">
         <v>48</v>
       </c>
-      <c r="Z29" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC29" t="s">
+      <c r="AD29" t="s">
         <v>49</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>50</v>
       </c>
       <c r="AE29" t="s">
         <v>15</v>
@@ -3808,13 +3809,13 @@
     </row>
     <row r="30" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D30">
         <v>170</v>
@@ -3841,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="L30" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="M30" t="s">
         <v>32</v>
@@ -3865,37 +3866,37 @@
         <v>14</v>
       </c>
       <c r="T30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U30" t="s">
         <v>15</v>
       </c>
       <c r="V30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X30" t="s">
         <v>15</v>
       </c>
       <c r="Y30" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC30" t="s">
         <v>48</v>
       </c>
-      <c r="Z30" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC30" t="s">
+      <c r="AD30" t="s">
         <v>49</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>50</v>
       </c>
       <c r="AE30" t="s">
         <v>15</v>
@@ -3909,13 +3910,13 @@
     </row>
     <row r="31" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31">
         <v>170</v>
@@ -3942,7 +3943,7 @@
         <v>0</v>
       </c>
       <c r="L31" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="M31" t="s">
         <v>32</v>
@@ -3977,13 +3978,13 @@
     </row>
     <row r="32" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D32">
         <v>500</v>
@@ -4010,7 +4011,7 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="M32" t="s">
         <v>32</v>
@@ -4031,7 +4032,7 @@
         <v>27</v>
       </c>
       <c r="S32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T32" t="s">
         <v>15</v>

</xml_diff>